<commit_message>
lpi individual system report adding more rows to hw/sw sheets
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2177 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: cac366a1b86f50f15e3fecc9f799f59e870d9ad9
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="System Overview" sheetId="21" r:id="rId1"/>
@@ -825,6 +825,30 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="49" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -846,9 +870,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -864,28 +885,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="12" fillId="0" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="6" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -896,9 +899,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5200,23 +5200,23 @@
     <row r="1" spans="1:19" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:19" s="4" customFormat="1" ht="119.25" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="30" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="32"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="40"/>
       <c r="O2"/>
       <c r="P2"/>
       <c r="Q2"/>
@@ -5246,21 +5246,21 @@
     </row>
     <row r="4" spans="1:19" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
       <c r="O4"/>
       <c r="P4"/>
       <c r="Q4"/>
@@ -5303,23 +5303,23 @@
     </row>
     <row r="7" spans="1:19" s="4" customFormat="1" ht="119.25" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="30" t="s">
+      <c r="C7" s="35"/>
+      <c r="D7" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="32"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="40"/>
       <c r="O7"/>
       <c r="P7"/>
       <c r="Q7"/>
@@ -5341,21 +5341,21 @@
     </row>
     <row r="9" spans="1:19" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="50"/>
       <c r="O9"/>
       <c r="P9"/>
       <c r="Q9"/>
@@ -5364,31 +5364,31 @@
     </row>
     <row r="10" spans="1:19" s="8" customFormat="1" ht="14.25" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33" t="s">
+      <c r="C10" s="28"/>
+      <c r="D10" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="33" t="s">
+      <c r="E10" s="47"/>
+      <c r="F10" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="43" t="s">
+      <c r="G10" s="28"/>
+      <c r="H10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="44"/>
-      <c r="J10" s="33" t="s">
+      <c r="I10" s="30"/>
+      <c r="J10" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33" t="s">
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="N10" s="33"/>
+      <c r="N10" s="28"/>
       <c r="O10"/>
       <c r="P10"/>
       <c r="Q10"/>
@@ -5397,19 +5397,19 @@
     </row>
     <row r="11" spans="1:19" ht="27.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
       <c r="O11"/>
       <c r="P11"/>
       <c r="Q11"/>
@@ -5418,19 +5418,19 @@
     </row>
     <row r="12" spans="1:19" ht="42.75" customHeight="1">
       <c r="A12" s="5"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="40"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
       <c r="O12"/>
       <c r="P12"/>
       <c r="Q12"/>
@@ -5451,23 +5451,23 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="5"/>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="50" t="s">
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
@@ -5475,23 +5475,23 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="5"/>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="50" t="s">
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="50"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
@@ -5499,23 +5499,23 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="5"/>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="50" t="s">
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="50"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
@@ -5523,23 +5523,23 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="5"/>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="50" t="s">
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="50"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="50"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
@@ -5547,23 +5547,23 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="5"/>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="50" t="s">
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="50"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
@@ -5571,23 +5571,23 @@
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="5"/>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="50" t="s">
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="50"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
@@ -5655,18 +5655,8 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E19:N19"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E14:N14"/>
-    <mergeCell ref="E15:N15"/>
-    <mergeCell ref="E16:N16"/>
-    <mergeCell ref="E17:N17"/>
-    <mergeCell ref="E18:N18"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="D7:N7"/>
+    <mergeCell ref="B9:N9"/>
     <mergeCell ref="B10:C11"/>
     <mergeCell ref="H10:I11"/>
     <mergeCell ref="B12:C12"/>
@@ -5683,8 +5673,18 @@
     <mergeCell ref="J10:L11"/>
     <mergeCell ref="D10:E11"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:N7"/>
-    <mergeCell ref="B9:N9"/>
+    <mergeCell ref="E19:N19"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E14:N14"/>
+    <mergeCell ref="E15:N15"/>
+    <mergeCell ref="E16:N16"/>
+    <mergeCell ref="E17:N17"/>
+    <mergeCell ref="E18:N18"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5700,10 +5700,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A2:K90"/>
+  <dimension ref="A2:K114"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6069,50 +6069,50 @@
       <c r="F32" s="16"/>
       <c r="G32" s="17"/>
     </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="17"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="17"/>
+    </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" s="52"/>
-      <c r="C34" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="56"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="57"/>
-    </row>
-    <row r="35" spans="1:7" ht="32.25" customHeight="1">
-      <c r="A35" s="53"/>
-      <c r="B35" s="54"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="59"/>
-      <c r="E35" s="59"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="60"/>
-    </row>
-    <row r="37" spans="1:7" ht="25.5">
-      <c r="A37" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>33</v>
-      </c>
+      <c r="A34" s="17"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="17"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="17"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="17"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="17"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="17"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="17"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="17"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="17"/>
@@ -6141,50 +6141,50 @@
       <c r="F40" s="16"/>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="17"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="17"/>
-    </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="17"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="17"/>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="17"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="17"/>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="17"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="17"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="17"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="17"/>
+      <c r="A42" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="52"/>
+      <c r="C42" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="57"/>
+    </row>
+    <row r="43" spans="1:7" ht="32.25" customHeight="1">
+      <c r="A43" s="53"/>
+      <c r="B43" s="54"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="59"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="60"/>
+    </row>
+    <row r="45" spans="1:7" ht="25.5">
+      <c r="A45" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="17"/>
@@ -6330,50 +6330,50 @@
       <c r="F61" s="16"/>
       <c r="G61" s="17"/>
     </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="17"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="17"/>
+    </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="B63" s="52"/>
-      <c r="C63" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="D63" s="56"/>
-      <c r="E63" s="56"/>
-      <c r="F63" s="56"/>
-      <c r="G63" s="57"/>
-    </row>
-    <row r="64" spans="1:7" ht="31.5" customHeight="1">
-      <c r="A64" s="53"/>
-      <c r="B64" s="54"/>
-      <c r="C64" s="58"/>
-      <c r="D64" s="59"/>
-      <c r="E64" s="59"/>
-      <c r="F64" s="59"/>
-      <c r="G64" s="60"/>
-    </row>
-    <row r="66" spans="1:7" ht="25.5">
-      <c r="A66" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B66" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C66" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D66" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E66" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F66" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G66" s="18" t="s">
-        <v>33</v>
-      </c>
+      <c r="A63" s="17"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="17"/>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="17"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="17"/>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="17"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="17"/>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="17"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="17"/>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="17"/>
@@ -6474,50 +6474,50 @@
       <c r="F77" s="16"/>
       <c r="G77" s="17"/>
     </row>
-    <row r="78" spans="1:7">
-      <c r="A78" s="17"/>
-      <c r="B78" s="15"/>
-      <c r="C78" s="16"/>
-      <c r="D78" s="17"/>
-      <c r="E78" s="15"/>
-      <c r="F78" s="16"/>
-      <c r="G78" s="17"/>
-    </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="17"/>
-      <c r="B79" s="15"/>
-      <c r="C79" s="16"/>
-      <c r="D79" s="17"/>
-      <c r="E79" s="15"/>
-      <c r="F79" s="16"/>
-      <c r="G79" s="17"/>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80" s="17"/>
-      <c r="B80" s="15"/>
-      <c r="C80" s="16"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="15"/>
-      <c r="F80" s="16"/>
-      <c r="G80" s="17"/>
-    </row>
-    <row r="81" spans="1:7">
-      <c r="A81" s="17"/>
-      <c r="B81" s="15"/>
-      <c r="C81" s="16"/>
-      <c r="D81" s="17"/>
-      <c r="E81" s="15"/>
-      <c r="F81" s="16"/>
-      <c r="G81" s="17"/>
-    </row>
-    <row r="82" spans="1:7">
-      <c r="A82" s="17"/>
-      <c r="B82" s="15"/>
-      <c r="C82" s="16"/>
-      <c r="D82" s="17"/>
-      <c r="E82" s="15"/>
-      <c r="F82" s="16"/>
-      <c r="G82" s="17"/>
+      <c r="A79" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B79" s="52"/>
+      <c r="C79" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="D79" s="56"/>
+      <c r="E79" s="56"/>
+      <c r="F79" s="56"/>
+      <c r="G79" s="57"/>
+    </row>
+    <row r="80" spans="1:7" ht="31.5" customHeight="1">
+      <c r="A80" s="53"/>
+      <c r="B80" s="54"/>
+      <c r="C80" s="58"/>
+      <c r="D80" s="59"/>
+      <c r="E80" s="59"/>
+      <c r="F80" s="59"/>
+      <c r="G80" s="60"/>
+    </row>
+    <row r="82" spans="1:7" ht="25.5">
+      <c r="A82" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B82" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D82" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E82" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F82" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G82" s="18" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="17"/>
@@ -6591,12 +6591,228 @@
       <c r="F90" s="16"/>
       <c r="G90" s="17"/>
     </row>
+    <row r="91" spans="1:7">
+      <c r="A91" s="17"/>
+      <c r="B91" s="15"/>
+      <c r="C91" s="16"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="15"/>
+      <c r="F91" s="16"/>
+      <c r="G91" s="17"/>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" s="17"/>
+      <c r="B92" s="15"/>
+      <c r="C92" s="16"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="15"/>
+      <c r="F92" s="16"/>
+      <c r="G92" s="17"/>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" s="17"/>
+      <c r="B93" s="15"/>
+      <c r="C93" s="16"/>
+      <c r="D93" s="17"/>
+      <c r="E93" s="15"/>
+      <c r="F93" s="16"/>
+      <c r="G93" s="17"/>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" s="17"/>
+      <c r="B94" s="15"/>
+      <c r="C94" s="16"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="15"/>
+      <c r="F94" s="16"/>
+      <c r="G94" s="17"/>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" s="17"/>
+      <c r="B95" s="15"/>
+      <c r="C95" s="16"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="16"/>
+      <c r="G95" s="17"/>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" s="17"/>
+      <c r="B96" s="15"/>
+      <c r="C96" s="16"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="15"/>
+      <c r="F96" s="16"/>
+      <c r="G96" s="17"/>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" s="17"/>
+      <c r="B97" s="15"/>
+      <c r="C97" s="16"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="15"/>
+      <c r="F97" s="16"/>
+      <c r="G97" s="17"/>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" s="17"/>
+      <c r="B98" s="15"/>
+      <c r="C98" s="16"/>
+      <c r="D98" s="17"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="16"/>
+      <c r="G98" s="17"/>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" s="17"/>
+      <c r="B99" s="15"/>
+      <c r="C99" s="16"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="15"/>
+      <c r="F99" s="16"/>
+      <c r="G99" s="17"/>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" s="17"/>
+      <c r="B100" s="15"/>
+      <c r="C100" s="16"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="15"/>
+      <c r="F100" s="16"/>
+      <c r="G100" s="17"/>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" s="17"/>
+      <c r="B101" s="15"/>
+      <c r="C101" s="16"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="15"/>
+      <c r="F101" s="16"/>
+      <c r="G101" s="17"/>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" s="17"/>
+      <c r="B102" s="15"/>
+      <c r="C102" s="16"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="15"/>
+      <c r="F102" s="16"/>
+      <c r="G102" s="17"/>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" s="17"/>
+      <c r="B103" s="15"/>
+      <c r="C103" s="16"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="15"/>
+      <c r="F103" s="16"/>
+      <c r="G103" s="17"/>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" s="17"/>
+      <c r="B104" s="15"/>
+      <c r="C104" s="16"/>
+      <c r="D104" s="17"/>
+      <c r="E104" s="15"/>
+      <c r="F104" s="16"/>
+      <c r="G104" s="17"/>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" s="17"/>
+      <c r="B105" s="15"/>
+      <c r="C105" s="16"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="15"/>
+      <c r="F105" s="16"/>
+      <c r="G105" s="17"/>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" s="17"/>
+      <c r="B106" s="15"/>
+      <c r="C106" s="16"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="15"/>
+      <c r="F106" s="16"/>
+      <c r="G106" s="17"/>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" s="17"/>
+      <c r="B107" s="15"/>
+      <c r="C107" s="16"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="15"/>
+      <c r="F107" s="16"/>
+      <c r="G107" s="17"/>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" s="17"/>
+      <c r="B108" s="15"/>
+      <c r="C108" s="16"/>
+      <c r="D108" s="17"/>
+      <c r="E108" s="15"/>
+      <c r="F108" s="16"/>
+      <c r="G108" s="17"/>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" s="17"/>
+      <c r="B109" s="15"/>
+      <c r="C109" s="16"/>
+      <c r="D109" s="17"/>
+      <c r="E109" s="15"/>
+      <c r="F109" s="16"/>
+      <c r="G109" s="17"/>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" s="17"/>
+      <c r="B110" s="15"/>
+      <c r="C110" s="16"/>
+      <c r="D110" s="17"/>
+      <c r="E110" s="15"/>
+      <c r="F110" s="16"/>
+      <c r="G110" s="17"/>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" s="17"/>
+      <c r="B111" s="15"/>
+      <c r="C111" s="16"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="15"/>
+      <c r="F111" s="16"/>
+      <c r="G111" s="17"/>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" s="17"/>
+      <c r="B112" s="15"/>
+      <c r="C112" s="16"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="15"/>
+      <c r="F112" s="16"/>
+      <c r="G112" s="17"/>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" s="17"/>
+      <c r="B113" s="15"/>
+      <c r="C113" s="16"/>
+      <c r="D113" s="17"/>
+      <c r="E113" s="15"/>
+      <c r="F113" s="16"/>
+      <c r="G113" s="17"/>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" s="17"/>
+      <c r="B114" s="15"/>
+      <c r="C114" s="16"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="15"/>
+      <c r="F114" s="16"/>
+      <c r="G114" s="17"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A34:B35"/>
-    <mergeCell ref="C34:G35"/>
-    <mergeCell ref="A63:B64"/>
-    <mergeCell ref="C63:G64"/>
+    <mergeCell ref="A42:B43"/>
+    <mergeCell ref="C42:G43"/>
+    <mergeCell ref="A79:B80"/>
+    <mergeCell ref="C79:G80"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="C5:G6"/>
     <mergeCell ref="A5:B6"/>
@@ -6612,10 +6828,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A2:K90"/>
+  <dimension ref="A2:K114"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6981,50 +7197,50 @@
       <c r="F32" s="16"/>
       <c r="G32" s="17"/>
     </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="17"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="17"/>
+    </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" s="52"/>
-      <c r="C34" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="56"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="57"/>
-    </row>
-    <row r="35" spans="1:7" ht="27" customHeight="1">
-      <c r="A35" s="53"/>
-      <c r="B35" s="54"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="59"/>
-      <c r="E35" s="59"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="60"/>
-    </row>
-    <row r="37" spans="1:7" ht="25.5">
-      <c r="A37" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>35</v>
-      </c>
+      <c r="A34" s="17"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="17"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="17"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="17"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="17"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="17"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="17"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="17"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="17"/>
@@ -7053,50 +7269,50 @@
       <c r="F40" s="16"/>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="17"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="17"/>
-    </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="17"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="17"/>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="17"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="17"/>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="17"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="17"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="17"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="17"/>
+      <c r="A42" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="52"/>
+      <c r="C42" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="57"/>
+    </row>
+    <row r="43" spans="1:7" ht="27" customHeight="1">
+      <c r="A43" s="53"/>
+      <c r="B43" s="54"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="59"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="60"/>
+    </row>
+    <row r="45" spans="1:7" ht="25.5">
+      <c r="A45" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="17"/>
@@ -7242,50 +7458,50 @@
       <c r="F61" s="16"/>
       <c r="G61" s="17"/>
     </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="17"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="17"/>
+    </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="B63" s="52"/>
-      <c r="C63" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="D63" s="56"/>
-      <c r="E63" s="56"/>
-      <c r="F63" s="56"/>
-      <c r="G63" s="57"/>
-    </row>
-    <row r="64" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A64" s="53"/>
-      <c r="B64" s="54"/>
-      <c r="C64" s="58"/>
-      <c r="D64" s="59"/>
-      <c r="E64" s="59"/>
-      <c r="F64" s="59"/>
-      <c r="G64" s="60"/>
-    </row>
-    <row r="66" spans="1:7" ht="25.5">
-      <c r="A66" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B66" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C66" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D66" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E66" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F66" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G66" s="18" t="s">
-        <v>35</v>
-      </c>
+      <c r="A63" s="17"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="17"/>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="17"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="17"/>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="17"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="17"/>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="17"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="17"/>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="17"/>
@@ -7386,50 +7602,50 @@
       <c r="F77" s="16"/>
       <c r="G77" s="17"/>
     </row>
-    <row r="78" spans="1:7">
-      <c r="A78" s="17"/>
-      <c r="B78" s="15"/>
-      <c r="C78" s="16"/>
-      <c r="D78" s="17"/>
-      <c r="E78" s="15"/>
-      <c r="F78" s="16"/>
-      <c r="G78" s="17"/>
-    </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="17"/>
-      <c r="B79" s="15"/>
-      <c r="C79" s="16"/>
-      <c r="D79" s="17"/>
-      <c r="E79" s="15"/>
-      <c r="F79" s="16"/>
-      <c r="G79" s="17"/>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80" s="17"/>
-      <c r="B80" s="15"/>
-      <c r="C80" s="16"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="15"/>
-      <c r="F80" s="16"/>
-      <c r="G80" s="17"/>
-    </row>
-    <row r="81" spans="1:7">
-      <c r="A81" s="17"/>
-      <c r="B81" s="15"/>
-      <c r="C81" s="16"/>
-      <c r="D81" s="17"/>
-      <c r="E81" s="15"/>
-      <c r="F81" s="16"/>
-      <c r="G81" s="17"/>
-    </row>
-    <row r="82" spans="1:7">
-      <c r="A82" s="17"/>
-      <c r="B82" s="15"/>
-      <c r="C82" s="16"/>
-      <c r="D82" s="17"/>
-      <c r="E82" s="15"/>
-      <c r="F82" s="16"/>
-      <c r="G82" s="17"/>
+      <c r="A79" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B79" s="52"/>
+      <c r="C79" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="D79" s="56"/>
+      <c r="E79" s="56"/>
+      <c r="F79" s="56"/>
+      <c r="G79" s="57"/>
+    </row>
+    <row r="80" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A80" s="53"/>
+      <c r="B80" s="54"/>
+      <c r="C80" s="58"/>
+      <c r="D80" s="59"/>
+      <c r="E80" s="59"/>
+      <c r="F80" s="59"/>
+      <c r="G80" s="60"/>
+    </row>
+    <row r="82" spans="1:7" ht="25.5">
+      <c r="A82" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B82" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D82" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E82" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F82" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G82" s="18" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="17"/>
@@ -7503,16 +7719,232 @@
       <c r="F90" s="16"/>
       <c r="G90" s="17"/>
     </row>
+    <row r="91" spans="1:7">
+      <c r="A91" s="17"/>
+      <c r="B91" s="15"/>
+      <c r="C91" s="16"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="15"/>
+      <c r="F91" s="16"/>
+      <c r="G91" s="17"/>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" s="17"/>
+      <c r="B92" s="15"/>
+      <c r="C92" s="16"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="15"/>
+      <c r="F92" s="16"/>
+      <c r="G92" s="17"/>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" s="17"/>
+      <c r="B93" s="15"/>
+      <c r="C93" s="16"/>
+      <c r="D93" s="17"/>
+      <c r="E93" s="15"/>
+      <c r="F93" s="16"/>
+      <c r="G93" s="17"/>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" s="17"/>
+      <c r="B94" s="15"/>
+      <c r="C94" s="16"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="15"/>
+      <c r="F94" s="16"/>
+      <c r="G94" s="17"/>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" s="17"/>
+      <c r="B95" s="15"/>
+      <c r="C95" s="16"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="16"/>
+      <c r="G95" s="17"/>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" s="17"/>
+      <c r="B96" s="15"/>
+      <c r="C96" s="16"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="15"/>
+      <c r="F96" s="16"/>
+      <c r="G96" s="17"/>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" s="17"/>
+      <c r="B97" s="15"/>
+      <c r="C97" s="16"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="15"/>
+      <c r="F97" s="16"/>
+      <c r="G97" s="17"/>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" s="17"/>
+      <c r="B98" s="15"/>
+      <c r="C98" s="16"/>
+      <c r="D98" s="17"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="16"/>
+      <c r="G98" s="17"/>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" s="17"/>
+      <c r="B99" s="15"/>
+      <c r="C99" s="16"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="15"/>
+      <c r="F99" s="16"/>
+      <c r="G99" s="17"/>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" s="17"/>
+      <c r="B100" s="15"/>
+      <c r="C100" s="16"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="15"/>
+      <c r="F100" s="16"/>
+      <c r="G100" s="17"/>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" s="17"/>
+      <c r="B101" s="15"/>
+      <c r="C101" s="16"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="15"/>
+      <c r="F101" s="16"/>
+      <c r="G101" s="17"/>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" s="17"/>
+      <c r="B102" s="15"/>
+      <c r="C102" s="16"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="15"/>
+      <c r="F102" s="16"/>
+      <c r="G102" s="17"/>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" s="17"/>
+      <c r="B103" s="15"/>
+      <c r="C103" s="16"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="15"/>
+      <c r="F103" s="16"/>
+      <c r="G103" s="17"/>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" s="17"/>
+      <c r="B104" s="15"/>
+      <c r="C104" s="16"/>
+      <c r="D104" s="17"/>
+      <c r="E104" s="15"/>
+      <c r="F104" s="16"/>
+      <c r="G104" s="17"/>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" s="17"/>
+      <c r="B105" s="15"/>
+      <c r="C105" s="16"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="15"/>
+      <c r="F105" s="16"/>
+      <c r="G105" s="17"/>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" s="17"/>
+      <c r="B106" s="15"/>
+      <c r="C106" s="16"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="15"/>
+      <c r="F106" s="16"/>
+      <c r="G106" s="17"/>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" s="17"/>
+      <c r="B107" s="15"/>
+      <c r="C107" s="16"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="15"/>
+      <c r="F107" s="16"/>
+      <c r="G107" s="17"/>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" s="17"/>
+      <c r="B108" s="15"/>
+      <c r="C108" s="16"/>
+      <c r="D108" s="17"/>
+      <c r="E108" s="15"/>
+      <c r="F108" s="16"/>
+      <c r="G108" s="17"/>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" s="17"/>
+      <c r="B109" s="15"/>
+      <c r="C109" s="16"/>
+      <c r="D109" s="17"/>
+      <c r="E109" s="15"/>
+      <c r="F109" s="16"/>
+      <c r="G109" s="17"/>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" s="17"/>
+      <c r="B110" s="15"/>
+      <c r="C110" s="16"/>
+      <c r="D110" s="17"/>
+      <c r="E110" s="15"/>
+      <c r="F110" s="16"/>
+      <c r="G110" s="17"/>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" s="17"/>
+      <c r="B111" s="15"/>
+      <c r="C111" s="16"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="15"/>
+      <c r="F111" s="16"/>
+      <c r="G111" s="17"/>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" s="17"/>
+      <c r="B112" s="15"/>
+      <c r="C112" s="16"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="15"/>
+      <c r="F112" s="16"/>
+      <c r="G112" s="17"/>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" s="17"/>
+      <c r="B113" s="15"/>
+      <c r="C113" s="16"/>
+      <c r="D113" s="17"/>
+      <c r="E113" s="15"/>
+      <c r="F113" s="16"/>
+      <c r="G113" s="17"/>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" s="17"/>
+      <c r="B114" s="15"/>
+      <c r="C114" s="16"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="15"/>
+      <c r="F114" s="16"/>
+      <c r="G114" s="17"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A63:B64"/>
-    <mergeCell ref="C63:G64"/>
+    <mergeCell ref="A79:B80"/>
+    <mergeCell ref="C79:G80"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A5:B6"/>
     <mergeCell ref="C5:G6"/>
-    <mergeCell ref="A34:B35"/>
-    <mergeCell ref="C34:G35"/>
+    <mergeCell ref="A42:B43"/>
+    <mergeCell ref="C42:G43"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
@@ -8053,8 +8485,8 @@
   </sheetPr>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
updated excel report for individual system transition
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2181 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 574f091901ddf22f00abb25189f380dcabeb46bd
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727"/>
   </bookViews>
   <sheets>
     <sheet name="System Overview" sheetId="21" r:id="rId1"/>
@@ -62,7 +62,7 @@
     <definedName name="ODS_SUM">'[2]POM 2 Enabler - FY12'!$M$102</definedName>
     <definedName name="Portal_ROI">[2]BOM!$N$46</definedName>
     <definedName name="Portal_SUM">'[2]POM 2 Enabler - FY12'!$N$102</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'System Overview'!$A$2:$R$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'System Overview'!$A$2:$R$12</definedName>
     <definedName name="Priority3">[4]Data1!$B$4:$B$6</definedName>
     <definedName name="ProcContractMonths">'[2]New Timeline'!$A$22</definedName>
     <definedName name="RangeBLU">[5]BLUBackEnd!$G$5:$G$49</definedName>
@@ -768,7 +768,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -825,11 +825,23 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="49" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -838,12 +850,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="12" fillId="0" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -859,15 +865,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -891,14 +888,11 @@
     <xf numFmtId="0" fontId="18" fillId="6" borderId="6" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5174,10 +5168,10 @@
     <tabColor theme="4" tint="-6.1037018951994385E-5"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:N7"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5200,23 +5194,23 @@
     <row r="1" spans="1:19" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:19" s="4" customFormat="1" ht="119.25" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="38" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="40"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="28"/>
       <c r="O2"/>
       <c r="P2"/>
       <c r="Q2"/>
@@ -5246,21 +5240,21 @@
     </row>
     <row r="4" spans="1:19" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
       <c r="O4"/>
       <c r="P4"/>
       <c r="Q4"/>
@@ -5303,23 +5297,23 @@
     </row>
     <row r="7" spans="1:19" s="4" customFormat="1" ht="119.25" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="38" t="s">
+      <c r="C7" s="37"/>
+      <c r="D7" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="40"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="28"/>
       <c r="O7"/>
       <c r="P7"/>
       <c r="Q7"/>
@@ -5341,133 +5335,136 @@
     </row>
     <row r="9" spans="1:19" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="50"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="31"/>
       <c r="O9"/>
       <c r="P9"/>
       <c r="Q9"/>
       <c r="R9"/>
       <c r="S9"/>
     </row>
-    <row r="10" spans="1:19" s="8" customFormat="1" ht="14.25" customHeight="1">
+    <row r="10" spans="1:19" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28" t="s">
+      <c r="C10" s="32"/>
+      <c r="D10" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="47"/>
-      <c r="F10" s="28" t="s">
+      <c r="E10" s="46"/>
+      <c r="F10" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="29" t="s">
+      <c r="G10" s="32"/>
+      <c r="H10" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="30"/>
-      <c r="J10" s="28" t="s">
+      <c r="I10" s="34"/>
+      <c r="J10" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28" t="s">
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="N10" s="28"/>
+      <c r="N10" s="32"/>
       <c r="O10"/>
       <c r="P10"/>
       <c r="Q10"/>
       <c r="R10"/>
       <c r="S10"/>
     </row>
-    <row r="11" spans="1:19" ht="27.75" customHeight="1">
+    <row r="11" spans="1:19" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="45"/>
       <c r="O11"/>
       <c r="P11"/>
       <c r="Q11"/>
       <c r="R11"/>
       <c r="S11"/>
     </row>
-    <row r="12" spans="1:19" ht="42.75" customHeight="1">
+    <row r="12" spans="1:19" ht="7.5" customHeight="1">
       <c r="A12" s="5"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="46"/>
-      <c r="N12" s="46"/>
-      <c r="O12"/>
-      <c r="P12"/>
-      <c r="Q12"/>
-      <c r="R12"/>
-      <c r="S12"/>
-    </row>
-    <row r="13" spans="1:19" ht="7.5" customHeight="1">
+      <c r="J12" s="5"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
+      <c r="B13" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="5"/>
-      <c r="B14" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="26" t="s">
+      <c r="B14" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
@@ -5475,23 +5472,23 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="5"/>
-      <c r="B15" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="26" t="s">
+      <c r="B15" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
@@ -5499,23 +5496,23 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="5"/>
-      <c r="B16" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="26" t="s">
+      <c r="B16" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
@@ -5523,23 +5520,23 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="5"/>
-      <c r="B17" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="26" t="s">
+      <c r="B17" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
@@ -5547,23 +5544,23 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="5"/>
-      <c r="B18" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="26" t="s">
+      <c r="B18" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="47"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
@@ -5571,23 +5568,19 @@
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="5"/>
-      <c r="B19" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
@@ -5633,58 +5626,38 @@
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
     </row>
-    <row r="22" spans="1:18">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-    </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="D7:N7"/>
-    <mergeCell ref="B9:N9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="H10:I11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B4:N4"/>
-    <mergeCell ref="D2:N2"/>
-    <mergeCell ref="F10:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="M10:N11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="J10:L11"/>
-    <mergeCell ref="D10:E11"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E19:N19"/>
+    <mergeCell ref="E18:N18"/>
+    <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E13:N13"/>
     <mergeCell ref="E14:N14"/>
     <mergeCell ref="E15:N15"/>
     <mergeCell ref="E16:N16"/>
     <mergeCell ref="E17:N17"/>
-    <mergeCell ref="E18:N18"/>
+    <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B4:N4"/>
+    <mergeCell ref="D2:N2"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:N7"/>
+    <mergeCell ref="B9:N9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5719,60 +5692,60 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="18" customHeight="1">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
     </row>
     <row r="3" spans="1:11" ht="18" customHeight="1">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
       <c r="H3"/>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="55" t="s">
+      <c r="B5" s="50"/>
+      <c r="C5" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="57"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="55"/>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
     </row>
     <row r="6" spans="1:11" ht="30.75" customHeight="1">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="60"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="58"/>
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
@@ -6142,26 +6115,26 @@
       <c r="G40" s="17"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="51" t="s">
+      <c r="A42" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="52"/>
-      <c r="C42" s="55" t="s">
+      <c r="B42" s="50"/>
+      <c r="C42" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="56"/>
-      <c r="E42" s="56"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="57"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="54"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="55"/>
     </row>
     <row r="43" spans="1:7" ht="32.25" customHeight="1">
-      <c r="A43" s="53"/>
-      <c r="B43" s="54"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="59"/>
-      <c r="E43" s="59"/>
-      <c r="F43" s="59"/>
-      <c r="G43" s="60"/>
+      <c r="A43" s="51"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="56"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="58"/>
     </row>
     <row r="45" spans="1:7" ht="25.5">
       <c r="A45" s="18" t="s">
@@ -6475,26 +6448,26 @@
       <c r="G77" s="17"/>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="51" t="s">
+      <c r="A79" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B79" s="52"/>
-      <c r="C79" s="55" t="s">
+      <c r="B79" s="50"/>
+      <c r="C79" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="D79" s="56"/>
-      <c r="E79" s="56"/>
-      <c r="F79" s="56"/>
-      <c r="G79" s="57"/>
+      <c r="D79" s="54"/>
+      <c r="E79" s="54"/>
+      <c r="F79" s="54"/>
+      <c r="G79" s="55"/>
     </row>
     <row r="80" spans="1:7" ht="31.5" customHeight="1">
-      <c r="A80" s="53"/>
-      <c r="B80" s="54"/>
-      <c r="C80" s="58"/>
-      <c r="D80" s="59"/>
-      <c r="E80" s="59"/>
-      <c r="F80" s="59"/>
-      <c r="G80" s="60"/>
+      <c r="A80" s="51"/>
+      <c r="B80" s="52"/>
+      <c r="C80" s="56"/>
+      <c r="D80" s="57"/>
+      <c r="E80" s="57"/>
+      <c r="F80" s="57"/>
+      <c r="G80" s="58"/>
     </row>
     <row r="82" spans="1:7" ht="25.5">
       <c r="A82" s="18" t="s">
@@ -6830,7 +6803,7 @@
   </sheetPr>
   <dimension ref="A2:K114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
@@ -6847,60 +6820,60 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="18" customHeight="1">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="65"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="63"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
     </row>
     <row r="3" spans="1:11" ht="18" customHeight="1">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
       <c r="H3"/>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="55" t="s">
+      <c r="B5" s="50"/>
+      <c r="C5" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="57"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="55"/>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
     </row>
     <row r="6" spans="1:11" ht="30.75" customHeight="1">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="60"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="58"/>
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
@@ -7270,26 +7243,26 @@
       <c r="G40" s="17"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="51" t="s">
+      <c r="A42" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="52"/>
-      <c r="C42" s="55" t="s">
+      <c r="B42" s="50"/>
+      <c r="C42" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="D42" s="56"/>
-      <c r="E42" s="56"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="57"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="54"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="55"/>
     </row>
     <row r="43" spans="1:7" ht="27" customHeight="1">
-      <c r="A43" s="53"/>
-      <c r="B43" s="54"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="59"/>
-      <c r="E43" s="59"/>
-      <c r="F43" s="59"/>
-      <c r="G43" s="60"/>
+      <c r="A43" s="51"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="56"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="58"/>
     </row>
     <row r="45" spans="1:7" ht="25.5">
       <c r="A45" s="18" t="s">
@@ -7603,26 +7576,26 @@
       <c r="G77" s="17"/>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="51" t="s">
+      <c r="A79" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B79" s="52"/>
-      <c r="C79" s="55" t="s">
+      <c r="B79" s="50"/>
+      <c r="C79" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="D79" s="56"/>
-      <c r="E79" s="56"/>
-      <c r="F79" s="56"/>
-      <c r="G79" s="57"/>
+      <c r="D79" s="54"/>
+      <c r="E79" s="54"/>
+      <c r="F79" s="54"/>
+      <c r="G79" s="55"/>
     </row>
     <row r="80" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A80" s="53"/>
-      <c r="B80" s="54"/>
-      <c r="C80" s="58"/>
-      <c r="D80" s="59"/>
-      <c r="E80" s="59"/>
-      <c r="F80" s="59"/>
-      <c r="G80" s="60"/>
+      <c r="A80" s="51"/>
+      <c r="B80" s="52"/>
+      <c r="C80" s="56"/>
+      <c r="D80" s="57"/>
+      <c r="E80" s="57"/>
+      <c r="F80" s="57"/>
+      <c r="G80" s="58"/>
     </row>
     <row r="82" spans="1:7" ht="25.5">
       <c r="A82" s="18" t="s">
@@ -7971,11 +7944,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="13"/>
@@ -7986,10 +7959,10 @@
       <c r="A4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="68"/>
+      <c r="C4" s="66"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -8156,10 +8129,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="66"/>
+      <c r="B2" s="64"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="13"/>
@@ -8311,11 +8284,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="13"/>
@@ -8326,10 +8299,10 @@
       <c r="A4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="68"/>
+      <c r="C4" s="66"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -8506,34 +8479,34 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18" customHeight="1"/>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
     </row>
     <row r="4" spans="1:11" ht="20.25" customHeight="1">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="69" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="71"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="69"/>
     </row>
     <row r="6" spans="1:11" ht="53.25" customHeight="1">
       <c r="A6" s="18" t="s">

</xml_diff>

<commit_message>
updated template for lpi system transition report
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2210 ef391c1c-ee15-45f7-b1d6-dde3d27a2169
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>System</t>
-  </si>
-  <si>
-    <t>LPI Report Overview</t>
   </si>
   <si>
     <t>System Information</t>
@@ -210,9 +207,6 @@
   </si>
   <si>
     <t>System Description</t>
-  </si>
-  <si>
-    <t>Description of LPI Report - provide an overview based upon the slide deck. [Static]</t>
   </si>
   <si>
     <t>System Data</t>
@@ -347,6 +341,14 @@
   </si>
   <si>
     <t>Explanation of what system is.</t>
+  </si>
+  <si>
+    <t>Report Overview</t>
+  </si>
+  <si>
+    <t>The Office of Transition Management (OTM) Transition Application Planning (TAP) coordinated with the Defense Health Clinical Systems (DHCS) and Defense Health Services Systems (DHSS) program offices, in addition to the tri-Services, to collect technical and functional data regarding their information systems, in order to fully characterize the legacy DHA IM/IT portfolio. 
+Using this data, OTM provided detailed analysis regarding each legacy system to the Functional Advisory Council (FAC), which made transition decisions that define if each system would be replaced by the future-state EHR (high probability systems) or would endure to support the future-state EHR (low probability systems).
+This report focuses on low probability systems that will require integration with the future-state EHR and provides analytical insights that specify the activities required for the system highlighted in this report to transition to the future state environment.</t>
   </si>
 </sst>
 </file>
@@ -803,6 +805,21 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="48" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -821,26 +838,17 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -916,12 +924,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -5127,7 +5129,7 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5145,24 +5147,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="7.5" customHeight="1"/>
-    <row r="2" spans="1:18" s="4" customFormat="1" ht="119.25" customHeight="1">
+    <row r="2" spans="1:18" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="37"/>
+      <c r="B2" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="29"/>
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
@@ -5191,20 +5193,20 @@
     </row>
     <row r="4" spans="1:18" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
+      <c r="B4" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
       <c r="N4"/>
       <c r="O4"/>
       <c r="P4"/>
@@ -5243,24 +5245,24 @@
       <c r="Q6"/>
       <c r="R6"/>
     </row>
-    <row r="7" spans="1:18" s="4" customFormat="1" ht="119.25" customHeight="1">
+    <row r="7" spans="1:18" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="37"/>
+      <c r="B7" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="29"/>
       <c r="N7"/>
       <c r="O7"/>
       <c r="P7"/>
@@ -5281,20 +5283,20 @@
     </row>
     <row r="9" spans="1:18" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="27"/>
+      <c r="B9" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="32"/>
       <c r="N9"/>
       <c r="O9"/>
       <c r="P9"/>
@@ -5303,30 +5305,30 @@
     </row>
     <row r="10" spans="1:18" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28" t="s">
+      <c r="C10" s="33"/>
+      <c r="D10" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="28" t="s">
+      <c r="G10" s="33"/>
+      <c r="H10" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="29" t="s">
+      <c r="I10" s="35"/>
+      <c r="J10" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="30"/>
-      <c r="J10" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28" t="s">
+      <c r="K10" s="33"/>
+      <c r="L10" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="28"/>
+      <c r="M10" s="33"/>
       <c r="N10"/>
       <c r="O10"/>
       <c r="P10"/>
@@ -5335,18 +5337,18 @@
     </row>
     <row r="11" spans="1:18" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="64"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="37"/>
       <c r="N11"/>
       <c r="O11"/>
       <c r="P11"/>
@@ -5355,11 +5357,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
@@ -5373,6 +5370,11 @@
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5407,60 +5409,60 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="18" customHeight="1">
-      <c r="A2" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
+      <c r="A2" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
     </row>
     <row r="3" spans="1:11" ht="18" customHeight="1">
-      <c r="A3" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
+      <c r="A3" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
       <c r="H3"/>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A5" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="45"/>
+      <c r="A5" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="42"/>
+      <c r="C5" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="47"/>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
     </row>
     <row r="6" spans="1:11" ht="30.75" customHeight="1">
-      <c r="A6" s="41"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="48"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="50"/>
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
@@ -5468,25 +5470,25 @@
     </row>
     <row r="8" spans="1:11" ht="26.25">
       <c r="A8" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="C8" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="17" t="s">
+      <c r="E8" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="F8" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="17" t="s">
-        <v>28</v>
-      </c>
       <c r="G8" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H8"/>
       <c r="I8"/>
@@ -5830,48 +5832,48 @@
       <c r="G40" s="16"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="B42" s="40"/>
-      <c r="C42" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="45"/>
+      <c r="A42" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="42"/>
+      <c r="C42" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="47"/>
     </row>
     <row r="43" spans="1:7" ht="32.25" customHeight="1">
-      <c r="A43" s="41"/>
-      <c r="B43" s="42"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="48"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="50"/>
     </row>
     <row r="45" spans="1:7" ht="25.5">
       <c r="A45" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="C45" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D45" s="17" t="s">
+      <c r="E45" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E45" s="17" t="s">
+      <c r="F45" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F45" s="17" t="s">
-        <v>28</v>
-      </c>
       <c r="G45" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -6163,48 +6165,48 @@
       <c r="G77" s="16"/>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="B79" s="40"/>
-      <c r="C79" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="D79" s="44"/>
-      <c r="E79" s="44"/>
-      <c r="F79" s="44"/>
-      <c r="G79" s="45"/>
+      <c r="A79" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B79" s="42"/>
+      <c r="C79" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D79" s="46"/>
+      <c r="E79" s="46"/>
+      <c r="F79" s="46"/>
+      <c r="G79" s="47"/>
     </row>
     <row r="80" spans="1:7" ht="31.5" customHeight="1">
-      <c r="A80" s="41"/>
-      <c r="B80" s="42"/>
-      <c r="C80" s="46"/>
-      <c r="D80" s="47"/>
-      <c r="E80" s="47"/>
-      <c r="F80" s="47"/>
-      <c r="G80" s="48"/>
+      <c r="A80" s="43"/>
+      <c r="B80" s="44"/>
+      <c r="C80" s="48"/>
+      <c r="D80" s="49"/>
+      <c r="E80" s="49"/>
+      <c r="F80" s="49"/>
+      <c r="G80" s="50"/>
     </row>
     <row r="82" spans="1:7" ht="25.5">
       <c r="A82" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B82" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B82" s="17" t="s">
+      <c r="C82" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D82" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C82" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D82" s="17" t="s">
+      <c r="E82" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E82" s="17" t="s">
+      <c r="F82" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F82" s="17" t="s">
-        <v>28</v>
-      </c>
       <c r="G82" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -6535,60 +6537,60 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="18" customHeight="1">
-      <c r="A2" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="53"/>
+      <c r="A2" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="55"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
     </row>
     <row r="3" spans="1:11" ht="18" customHeight="1">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
       <c r="H3"/>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A5" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="45"/>
+      <c r="A5" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="42"/>
+      <c r="C5" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="47"/>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
     </row>
     <row r="6" spans="1:11" ht="30.75" customHeight="1">
-      <c r="A6" s="41"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="48"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="50"/>
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
@@ -6596,25 +6598,25 @@
     </row>
     <row r="8" spans="1:11" ht="26.25">
       <c r="A8" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="17" t="s">
         <v>34</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>35</v>
       </c>
       <c r="H8"/>
       <c r="I8"/>
@@ -6958,48 +6960,48 @@
       <c r="G40" s="16"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="B42" s="40"/>
-      <c r="C42" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="45"/>
+      <c r="A42" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="42"/>
+      <c r="C42" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="47"/>
     </row>
     <row r="43" spans="1:7" ht="27" customHeight="1">
-      <c r="A43" s="41"/>
-      <c r="B43" s="42"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="48"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="50"/>
     </row>
     <row r="45" spans="1:7" ht="25.5">
       <c r="A45" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G45" s="17" t="s">
         <v>34</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -7291,48 +7293,48 @@
       <c r="G77" s="16"/>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="B79" s="40"/>
-      <c r="C79" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="D79" s="44"/>
-      <c r="E79" s="44"/>
-      <c r="F79" s="44"/>
-      <c r="G79" s="45"/>
+      <c r="A79" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B79" s="42"/>
+      <c r="C79" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D79" s="46"/>
+      <c r="E79" s="46"/>
+      <c r="F79" s="46"/>
+      <c r="G79" s="47"/>
     </row>
     <row r="80" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A80" s="41"/>
-      <c r="B80" s="42"/>
-      <c r="C80" s="46"/>
-      <c r="D80" s="47"/>
-      <c r="E80" s="47"/>
-      <c r="F80" s="47"/>
-      <c r="G80" s="48"/>
+      <c r="A80" s="43"/>
+      <c r="B80" s="44"/>
+      <c r="C80" s="48"/>
+      <c r="D80" s="49"/>
+      <c r="E80" s="49"/>
+      <c r="F80" s="49"/>
+      <c r="G80" s="50"/>
     </row>
     <row r="82" spans="1:7" ht="25.5">
       <c r="A82" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B82" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C82" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D82" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E82" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F82" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G82" s="17" t="s">
         <v>34</v>
-      </c>
-      <c r="B82" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C82" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D82" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E82" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F82" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G82" s="17" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -7659,11 +7661,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
+      <c r="A2" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -7674,10 +7676,10 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="56"/>
+      <c r="B4" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="58"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -7686,13 +7688,13 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -7844,10 +7846,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="54"/>
+      <c r="A2" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="56"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -7858,7 +7860,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4"/>
     </row>
@@ -7868,10 +7870,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -7999,11 +8001,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
+      <c r="A2" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -8014,10 +8016,10 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="56"/>
+      <c r="B4" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="58"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -8026,13 +8028,13 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -8194,65 +8196,65 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18" customHeight="1"/>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
+      <c r="A2" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
     </row>
     <row r="4" spans="1:11" ht="20.25" customHeight="1">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="59"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="61"/>
     </row>
     <row r="6" spans="1:11" ht="53.25" customHeight="1">
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="17" t="s">
+      <c r="E6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="17" t="s">
+      <c r="G6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="H6" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="I6" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="17" t="s">
         <v>21</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>22</v>
       </c>
       <c r="K6"/>
     </row>

</xml_diff>

<commit_message>
individual system transition modernization timeline
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2220 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: f24321e4db88c3eacdb901ff2566fc4e8c39ce68
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="System Overview" sheetId="21" r:id="rId1"/>
     <sheet name="Software Lifecycles" sheetId="22" r:id="rId2"/>
     <sheet name="Hardware Lifecycles" sheetId="23" r:id="rId3"/>
-    <sheet name="System Data" sheetId="24" r:id="rId4"/>
-    <sheet name="Data Provenance" sheetId="28" r:id="rId5"/>
-    <sheet name="DHMSM Data Requirements" sheetId="26" r:id="rId6"/>
-    <sheet name="System Interfaces" sheetId="27" r:id="rId7"/>
+    <sheet name="Modernization Timeline" sheetId="29" r:id="rId4"/>
+    <sheet name="System Data" sheetId="24" r:id="rId5"/>
+    <sheet name="Data Provenance" sheetId="28" r:id="rId6"/>
+    <sheet name="DHMSM Data Requirements" sheetId="26" r:id="rId7"/>
+    <sheet name="System Interfaces" sheetId="27" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
@@ -29,6 +29,7 @@
     <externalReference r:id="rId13"/>
     <externalReference r:id="rId14"/>
     <externalReference r:id="rId15"/>
+    <externalReference r:id="rId16"/>
   </externalReferences>
   <definedNames>
     <definedName name="Additional">[1]Data!$D$3:$D$15</definedName>
@@ -51,6 +52,7 @@
     <definedName name="FY13_Total">'[2]Fiscal Year Breakdown'!$AM$18</definedName>
     <definedName name="FY14_Total">'[2]Fiscal Year Breakdown'!$AN$18</definedName>
     <definedName name="FY15_Total">'[2]Fiscal Year Breakdown'!$AO$18</definedName>
+    <definedName name="I_O" localSheetId="3">#REF!</definedName>
     <definedName name="I_O" localSheetId="0">#REF!</definedName>
     <definedName name="I_O">#REF!</definedName>
     <definedName name="Link3">[4]Data1!$D$4:$D$182</definedName>
@@ -76,6 +78,7 @@
     <definedName name="SSO_ROI">[2]BOM!$N$54</definedName>
     <definedName name="StartDate">'[2]New Timeline'!$A$25</definedName>
     <definedName name="Teams">[2]Cheat!$A$38:$A$39</definedName>
+    <definedName name="Type" localSheetId="3">#REF!</definedName>
     <definedName name="Type" localSheetId="0">#REF!</definedName>
     <definedName name="Type">#REF!</definedName>
     <definedName name="UDDI_ROI">[2]BOM!$N$58</definedName>
@@ -87,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
   <si>
     <t>Garrison / Theater</t>
   </si>
@@ -349,6 +352,18 @@
     <t>The Office of Transition Management (OTM) Transition Application Planning (TAP) coordinated with the Defense Health Clinical Systems (DHCS) and Defense Health Services Systems (DHSS) program offices, in addition to the tri-Services, to collect technical and functional data regarding their information systems, in order to fully characterize the legacy DHA IM/IT portfolio. 
 Using this data, OTM provided detailed analysis regarding each legacy system to the Functional Advisory Council (FAC), which made transition decisions that define if each system would be replaced by the future-state EHR (high probability systems) or would endure to support the future-state EHR (low probability systems).
 This report focuses on low probability systems that will require integration with the future-state EHR and provides analytical insights that specify the activities required for the system highlighted in this report to transition to the future state environment.</t>
+  </si>
+  <si>
+    <t>System Modernization Timeline</t>
+  </si>
+  <si>
+    <t>This section displays the cost to upgrade software and hardware that @SYSTEM@ uses as they retire.</t>
+  </si>
+  <si>
+    <t>Software Cost</t>
+  </si>
+  <si>
+    <t>Hardware Cost</t>
   </si>
 </sst>
 </file>
@@ -749,7 +764,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -805,29 +820,11 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="48" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -844,14 +841,38 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -898,13 +919,16 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5128,8 +5152,8 @@
   </sheetPr>
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5149,22 +5173,22 @@
     <row r="1" spans="1:18" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:18" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="27" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="29"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="38"/>
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
@@ -5193,20 +5217,20 @@
     </row>
     <row r="4" spans="1:18" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
       <c r="N4"/>
       <c r="O4"/>
       <c r="P4"/>
@@ -5247,22 +5271,22 @@
     </row>
     <row r="7" spans="1:18" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="29"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="38"/>
       <c r="N7"/>
       <c r="O7"/>
       <c r="P7"/>
@@ -5283,20 +5307,20 @@
     </row>
     <row r="9" spans="1:18" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="32"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="42"/>
       <c r="N9"/>
       <c r="O9"/>
       <c r="P9"/>
@@ -5305,30 +5329,30 @@
     </row>
     <row r="10" spans="1:18" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33" t="s">
+      <c r="C10" s="27"/>
+      <c r="D10" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="33" t="s">
+      <c r="E10" s="39"/>
+      <c r="F10" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="34" t="s">
+      <c r="G10" s="27"/>
+      <c r="H10" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="35"/>
-      <c r="J10" s="33" t="s">
+      <c r="I10" s="29"/>
+      <c r="J10" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33" t="s">
+      <c r="K10" s="27"/>
+      <c r="L10" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="33"/>
+      <c r="M10" s="27"/>
       <c r="N10"/>
       <c r="O10"/>
       <c r="P10"/>
@@ -5337,18 +5361,18 @@
     </row>
     <row r="11" spans="1:18" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="37"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="31"/>
       <c r="N11"/>
       <c r="O11"/>
       <c r="P11"/>
@@ -5357,6 +5381,10 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
@@ -5371,10 +5399,6 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5409,60 +5433,60 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="18" customHeight="1">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
     </row>
     <row r="3" spans="1:11" ht="18" customHeight="1">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
       <c r="H3"/>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="45" t="s">
+      <c r="B5" s="44"/>
+      <c r="C5" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="47"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="49"/>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
     </row>
     <row r="6" spans="1:11" ht="30.75" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="50"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="52"/>
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
@@ -5832,26 +5856,26 @@
       <c r="G40" s="16"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="45" t="s">
+      <c r="B42" s="44"/>
+      <c r="C42" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="47"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="49"/>
     </row>
     <row r="43" spans="1:7" ht="32.25" customHeight="1">
-      <c r="A43" s="43"/>
-      <c r="B43" s="44"/>
-      <c r="C43" s="48"/>
-      <c r="D43" s="49"/>
-      <c r="E43" s="49"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="50"/>
+      <c r="A43" s="45"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="52"/>
     </row>
     <row r="45" spans="1:7" ht="25.5">
       <c r="A45" s="17" t="s">
@@ -6165,26 +6189,26 @@
       <c r="G77" s="16"/>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="41" t="s">
+      <c r="A79" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B79" s="42"/>
-      <c r="C79" s="45" t="s">
+      <c r="B79" s="44"/>
+      <c r="C79" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="D79" s="46"/>
-      <c r="E79" s="46"/>
-      <c r="F79" s="46"/>
-      <c r="G79" s="47"/>
+      <c r="D79" s="48"/>
+      <c r="E79" s="48"/>
+      <c r="F79" s="48"/>
+      <c r="G79" s="49"/>
     </row>
     <row r="80" spans="1:7" ht="31.5" customHeight="1">
-      <c r="A80" s="43"/>
-      <c r="B80" s="44"/>
-      <c r="C80" s="48"/>
-      <c r="D80" s="49"/>
-      <c r="E80" s="49"/>
-      <c r="F80" s="49"/>
-      <c r="G80" s="50"/>
+      <c r="A80" s="45"/>
+      <c r="B80" s="46"/>
+      <c r="C80" s="50"/>
+      <c r="D80" s="51"/>
+      <c r="E80" s="51"/>
+      <c r="F80" s="51"/>
+      <c r="G80" s="52"/>
     </row>
     <row r="82" spans="1:7" ht="25.5">
       <c r="A82" s="17" t="s">
@@ -6520,8 +6544,8 @@
   </sheetPr>
   <dimension ref="A2:K114"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6537,60 +6561,60 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="18" customHeight="1">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="55"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="57"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
     </row>
     <row r="3" spans="1:11" ht="18" customHeight="1">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
       <c r="H3"/>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="45" t="s">
+      <c r="B5" s="44"/>
+      <c r="C5" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="47"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="49"/>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
     </row>
     <row r="6" spans="1:11" ht="30.75" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="50"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="52"/>
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
@@ -6960,26 +6984,26 @@
       <c r="G40" s="16"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="45" t="s">
+      <c r="B42" s="44"/>
+      <c r="C42" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="47"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="49"/>
     </row>
     <row r="43" spans="1:7" ht="27" customHeight="1">
-      <c r="A43" s="43"/>
-      <c r="B43" s="44"/>
-      <c r="C43" s="48"/>
-      <c r="D43" s="49"/>
-      <c r="E43" s="49"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="50"/>
+      <c r="A43" s="45"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="52"/>
     </row>
     <row r="45" spans="1:7" ht="25.5">
       <c r="A45" s="17" t="s">
@@ -7293,26 +7317,26 @@
       <c r="G77" s="16"/>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="41" t="s">
+      <c r="A79" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B79" s="42"/>
-      <c r="C79" s="45" t="s">
+      <c r="B79" s="44"/>
+      <c r="C79" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="D79" s="46"/>
-      <c r="E79" s="46"/>
-      <c r="F79" s="46"/>
-      <c r="G79" s="47"/>
+      <c r="D79" s="48"/>
+      <c r="E79" s="48"/>
+      <c r="F79" s="48"/>
+      <c r="G79" s="49"/>
     </row>
     <row r="80" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A80" s="43"/>
-      <c r="B80" s="44"/>
-      <c r="C80" s="48"/>
-      <c r="D80" s="49"/>
-      <c r="E80" s="49"/>
-      <c r="F80" s="49"/>
-      <c r="G80" s="50"/>
+      <c r="A80" s="45"/>
+      <c r="B80" s="46"/>
+      <c r="C80" s="50"/>
+      <c r="D80" s="51"/>
+      <c r="E80" s="51"/>
+      <c r="F80" s="51"/>
+      <c r="G80" s="52"/>
     </row>
     <row r="82" spans="1:7" ht="25.5">
       <c r="A82" s="17" t="s">
@@ -7646,10 +7670,158 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
+  <dimension ref="A2:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
+    <col min="2" max="9" width="10.7109375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" ht="18">
+      <c r="A2" s="61" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+    </row>
+    <row r="3" spans="1:9" ht="18">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+    </row>
+    <row r="4" spans="1:9" ht="32.25" customHeight="1">
+      <c r="A4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="60"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" ht="24" customHeight="1">
+      <c r="B6" s="25">
+        <v>2015</v>
+      </c>
+      <c r="C6" s="25">
+        <v>2016</v>
+      </c>
+      <c r="D6" s="25">
+        <v>2017</v>
+      </c>
+      <c r="E6" s="25">
+        <v>2018</v>
+      </c>
+      <c r="F6" s="25">
+        <v>2019</v>
+      </c>
+      <c r="G6" s="25">
+        <v>2020</v>
+      </c>
+      <c r="H6" s="25">
+        <v>2021</v>
+      </c>
+      <c r="I6" s="25">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="24" customHeight="1">
+      <c r="A7" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="26">
+        <v>0</v>
+      </c>
+      <c r="C7" s="26">
+        <v>0</v>
+      </c>
+      <c r="D7" s="26">
+        <v>0</v>
+      </c>
+      <c r="E7" s="26">
+        <v>0</v>
+      </c>
+      <c r="F7" s="26">
+        <v>0</v>
+      </c>
+      <c r="G7" s="26">
+        <v>0</v>
+      </c>
+      <c r="H7" s="26">
+        <v>0</v>
+      </c>
+      <c r="I7" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="24" customHeight="1">
+      <c r="A8" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="26">
+        <v>0</v>
+      </c>
+      <c r="C8" s="26">
+        <v>0</v>
+      </c>
+      <c r="D8" s="26">
+        <v>0</v>
+      </c>
+      <c r="E8" s="26">
+        <v>0</v>
+      </c>
+      <c r="F8" s="26">
+        <v>0</v>
+      </c>
+      <c r="G8" s="26">
+        <v>0</v>
+      </c>
+      <c r="H8" s="26">
+        <v>0</v>
+      </c>
+      <c r="I8" s="26">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="A2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
   <dimension ref="A2:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7661,11 +7833,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -7676,10 +7848,10 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="58"/>
+      <c r="C4" s="60"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -7827,7 +7999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4"/>
@@ -7846,10 +8018,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="56"/>
+      <c r="B2" s="61"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -7981,7 +8153,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4"/>
@@ -8001,11 +8173,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -8016,10 +8188,10 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="58"/>
+      <c r="C4" s="60"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -8168,7 +8340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4"/>
@@ -8196,34 +8368,34 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18" customHeight="1"/>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
     </row>
     <row r="4" spans="1:11" ht="20.25" customHeight="1">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="59" t="s">
+      <c r="B4" s="66"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="61"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="64"/>
     </row>
     <row r="6" spans="1:11" ht="53.25" customHeight="1">
       <c r="A6" s="17" t="s">

</xml_diff>

<commit_message>
Updated system interfaces tab to include cost
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2229 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: d4ee1d12d0727037eba9dc15f43897b8ffaa7508
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmart\workspace64bitNew\SEMOSS_2014\export\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvenkataraman\Desktop\workspace\SEMOSS\export\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="System Overview" sheetId="21" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
   <si>
     <t>Garrison / Theater</t>
   </si>
@@ -337,9 +337,6 @@
     </r>
   </si>
   <si>
-    <t>This section displays the current @SYSTEM@ interfaces and how they are affected by DHMSM deployment</t>
-  </si>
-  <si>
     <t>System Name</t>
   </si>
   <si>
@@ -367,6 +364,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>This section displays the current @SYSTEM@ interfaces and how they are affected by DHMSM deployment.</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
@@ -829,39 +832,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -874,7 +844,40 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5176,22 +5179,22 @@
     <row r="1" spans="1:18" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:18" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="29"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="33"/>
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
@@ -5220,20 +5223,20 @@
     </row>
     <row r="4" spans="1:18" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
+      <c r="B4" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
       <c r="N4"/>
       <c r="O4"/>
       <c r="P4"/>
@@ -5274,22 +5277,22 @@
     </row>
     <row r="7" spans="1:18" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="29"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="33"/>
       <c r="N7"/>
       <c r="O7"/>
       <c r="P7"/>
@@ -5310,20 +5313,20 @@
     </row>
     <row r="9" spans="1:18" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="32"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="40"/>
       <c r="N9"/>
       <c r="O9"/>
       <c r="P9"/>
@@ -5332,30 +5335,30 @@
     </row>
     <row r="10" spans="1:18" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33" t="s">
+      <c r="C10" s="34"/>
+      <c r="D10" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="33" t="s">
+      <c r="E10" s="37"/>
+      <c r="F10" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="34" t="s">
+      <c r="G10" s="34"/>
+      <c r="H10" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="35"/>
-      <c r="J10" s="33" t="s">
+      <c r="I10" s="42"/>
+      <c r="J10" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33" t="s">
+      <c r="K10" s="34"/>
+      <c r="L10" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="33"/>
+      <c r="M10" s="34"/>
       <c r="N10"/>
       <c r="O10"/>
       <c r="P10"/>
@@ -5364,18 +5367,18 @@
     </row>
     <row r="11" spans="1:18" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="37"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="36"/>
       <c r="N11"/>
       <c r="O11"/>
       <c r="P11"/>
@@ -5384,6 +5387,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -5400,8 +5405,6 @@
     <mergeCell ref="D7:M7"/>
     <mergeCell ref="B9:M9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7675,8 +7678,8 @@
   </sheetPr>
   <dimension ref="A2:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7686,9 +7689,9 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="18">
+    <row r="2" spans="1:10" ht="18" customHeight="1">
       <c r="A2" s="61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="61"/>
       <c r="C2" s="61"/>
@@ -7698,6 +7701,7 @@
       <c r="G2" s="61"/>
       <c r="H2" s="61"/>
       <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="18">
       <c r="A3" s="12"/>
@@ -7708,7 +7712,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="59"/>
       <c r="D4" s="59"/>
@@ -7716,7 +7720,8 @@
       <c r="F4" s="59"/>
       <c r="G4" s="59"/>
       <c r="H4" s="59"/>
-      <c r="I4" s="60"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="2"/>
@@ -7748,12 +7753,12 @@
         <v>2022</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="24" customHeight="1">
       <c r="A7" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="26">
         <v>0</v>
@@ -7785,7 +7790,7 @@
     </row>
     <row r="8" spans="1:10" ht="24" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="26">
         <v>0</v>
@@ -7817,8 +7822,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
@@ -8359,8 +8364,8 @@
   </sheetPr>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8375,11 +8380,12 @@
     <col min="8" max="8" width="10.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="25.140625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="19.28515625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" customHeight="1"/>
-    <row r="2" spans="1:11" ht="18">
+    <row r="2" spans="1:11" ht="18" customHeight="1">
       <c r="A2" s="61" t="s">
         <v>42</v>
       </c>
@@ -8392,6 +8398,7 @@
       <c r="H2" s="61"/>
       <c r="I2" s="61"/>
       <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
     </row>
     <row r="4" spans="1:11" ht="20.25" customHeight="1">
       <c r="A4" s="65" t="s">
@@ -8400,14 +8407,15 @@
       <c r="B4" s="66"/>
       <c r="C4" s="67"/>
       <c r="D4" s="62" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E4" s="63"/>
       <c r="F4" s="63"/>
       <c r="G4" s="63"/>
       <c r="H4" s="63"/>
       <c r="I4" s="63"/>
-      <c r="J4" s="64"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="64"/>
     </row>
     <row r="6" spans="1:11" ht="53.25" customHeight="1">
       <c r="A6" s="17" t="s">
@@ -8440,9 +8448,11 @@
       <c r="J6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="K6"/>
-    </row>
-    <row r="7" spans="1:11" ht="15">
+      <c r="K6" s="17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
@@ -8453,9 +8463,9 @@
       <c r="H7" s="15"/>
       <c r="I7" s="16"/>
       <c r="J7" s="14"/>
-      <c r="K7"/>
-    </row>
-    <row r="8" spans="1:11" ht="15">
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
       <c r="C8" s="16"/>
@@ -8466,9 +8476,9 @@
       <c r="H8" s="15"/>
       <c r="I8" s="16"/>
       <c r="J8" s="14"/>
-      <c r="K8"/>
-    </row>
-    <row r="9" spans="1:11" ht="15">
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
       <c r="C9" s="16"/>
@@ -8479,9 +8489,9 @@
       <c r="H9" s="15"/>
       <c r="I9" s="16"/>
       <c r="J9" s="14"/>
-      <c r="K9"/>
-    </row>
-    <row r="10" spans="1:11" ht="15">
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
@@ -8492,9 +8502,9 @@
       <c r="H10" s="15"/>
       <c r="I10" s="16"/>
       <c r="J10" s="14"/>
-      <c r="K10"/>
-    </row>
-    <row r="11" spans="1:11" ht="15">
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
       <c r="C11" s="16"/>
@@ -8505,9 +8515,9 @@
       <c r="H11" s="15"/>
       <c r="I11" s="16"/>
       <c r="J11" s="14"/>
-      <c r="K11"/>
-    </row>
-    <row r="12" spans="1:11" ht="15">
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="14"/>
       <c r="B12" s="15"/>
       <c r="C12" s="16"/>
@@ -8518,9 +8528,9 @@
       <c r="H12" s="15"/>
       <c r="I12" s="16"/>
       <c r="J12" s="14"/>
-      <c r="K12"/>
-    </row>
-    <row r="13" spans="1:11" ht="15">
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="14"/>
       <c r="B13" s="15"/>
       <c r="C13" s="16"/>
@@ -8531,9 +8541,9 @@
       <c r="H13" s="15"/>
       <c r="I13" s="16"/>
       <c r="J13" s="14"/>
-      <c r="K13"/>
-    </row>
-    <row r="14" spans="1:11" ht="15">
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
@@ -8544,9 +8554,9 @@
       <c r="H14" s="15"/>
       <c r="I14" s="16"/>
       <c r="J14" s="14"/>
-      <c r="K14"/>
-    </row>
-    <row r="15" spans="1:11" ht="15">
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
@@ -8557,9 +8567,9 @@
       <c r="H15" s="15"/>
       <c r="I15" s="16"/>
       <c r="J15" s="14"/>
-      <c r="K15"/>
-    </row>
-    <row r="16" spans="1:11" ht="15">
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
@@ -8570,9 +8580,9 @@
       <c r="H16" s="15"/>
       <c r="I16" s="16"/>
       <c r="J16" s="14"/>
-      <c r="K16"/>
-    </row>
-    <row r="17" spans="1:11" ht="15">
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
@@ -8583,9 +8593,9 @@
       <c r="H17" s="15"/>
       <c r="I17" s="16"/>
       <c r="J17" s="14"/>
-      <c r="K17"/>
-    </row>
-    <row r="18" spans="1:11" ht="15">
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -8596,13 +8606,13 @@
       <c r="H18" s="15"/>
       <c r="I18" s="16"/>
       <c r="J18" s="14"/>
-      <c r="K18"/>
+      <c r="K18" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D4:J4"/>
-    <mergeCell ref="A2:J2"/>
     <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="D4:K4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
added extra column to show services
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2269 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 80f432ce8e1991f8257637d726a30607ad8163f0
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvenkataraman\Desktop\workspace\SEMOSS\export\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahkhalil\newWorkspace\Semoss\export\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
   <si>
     <t>Garrison / Theater</t>
   </si>
@@ -832,6 +832,18 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -856,12 +868,6 @@
     <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -873,12 +879,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -931,10 +931,19 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -945,15 +954,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -5179,22 +5179,22 @@
     <row r="1" spans="1:18" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:18" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="31" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="33"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="37"/>
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
@@ -5223,20 +5223,20 @@
     </row>
     <row r="4" spans="1:18" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
       <c r="N4"/>
       <c r="O4"/>
       <c r="P4"/>
@@ -5277,22 +5277,22 @@
     </row>
     <row r="7" spans="1:18" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="31" t="s">
+      <c r="C7" s="32"/>
+      <c r="D7" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="33"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="37"/>
       <c r="N7"/>
       <c r="O7"/>
       <c r="P7"/>
@@ -5313,20 +5313,20 @@
     </row>
     <row r="9" spans="1:18" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="40"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="42"/>
       <c r="N9"/>
       <c r="O9"/>
       <c r="P9"/>
@@ -5335,30 +5335,30 @@
     </row>
     <row r="10" spans="1:18" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34" t="s">
+      <c r="C10" s="38"/>
+      <c r="D10" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="37"/>
-      <c r="F10" s="34" t="s">
+      <c r="E10" s="39"/>
+      <c r="F10" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="41" t="s">
+      <c r="G10" s="38"/>
+      <c r="H10" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="42"/>
-      <c r="J10" s="34" t="s">
+      <c r="I10" s="28"/>
+      <c r="J10" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34" t="s">
+      <c r="K10" s="38"/>
+      <c r="L10" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="34"/>
+      <c r="M10" s="38"/>
       <c r="N10"/>
       <c r="O10"/>
       <c r="P10"/>
@@ -5367,18 +5367,18 @@
     </row>
     <row r="11" spans="1:18" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="36"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="30"/>
       <c r="N11"/>
       <c r="O11"/>
       <c r="P11"/>
@@ -5387,6 +5387,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
@@ -5403,8 +5405,6 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7690,18 +7690,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
     </row>
     <row r="3" spans="1:10" ht="18">
       <c r="A3" s="12"/>
@@ -7850,11 +7850,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -7868,7 +7868,7 @@
       <c r="B4" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="60"/>
+      <c r="C4" s="61"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -8035,10 +8035,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="61"/>
+      <c r="B2" s="60"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -8190,11 +8190,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -8208,7 +8208,7 @@
       <c r="B4" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="60"/>
+      <c r="C4" s="61"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -8362,10 +8362,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8378,46 +8378,48 @@
     <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="10" width="18.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" customHeight="1"/>
-    <row r="2" spans="1:11" ht="18" customHeight="1">
-      <c r="A2" s="61" t="s">
+    <row r="1" spans="1:12" ht="18" customHeight="1"/>
+    <row r="2" spans="1:12" ht="18" customHeight="1">
+      <c r="A2" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-    </row>
-    <row r="4" spans="1:11" ht="20.25" customHeight="1">
-      <c r="A4" s="65" t="s">
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+    </row>
+    <row r="4" spans="1:12" ht="20.25" customHeight="1">
+      <c r="A4" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="62" t="s">
+      <c r="B4" s="63"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="64"/>
-    </row>
-    <row r="6" spans="1:11" ht="53.25" customHeight="1">
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="67"/>
+    </row>
+    <row r="6" spans="1:12" ht="53.25" customHeight="1">
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
@@ -8446,13 +8448,16 @@
         <v>38</v>
       </c>
       <c r="J6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="L6" s="17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
@@ -8462,10 +8467,11 @@
       <c r="G7" s="14"/>
       <c r="H7" s="15"/>
       <c r="I7" s="16"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="15"/>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="J7" s="16"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="15"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
       <c r="C8" s="16"/>
@@ -8475,10 +8481,11 @@
       <c r="G8" s="14"/>
       <c r="H8" s="15"/>
       <c r="I8" s="16"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="15"/>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="J8" s="16"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="15"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
       <c r="C9" s="16"/>
@@ -8488,10 +8495,11 @@
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
       <c r="I9" s="16"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="15"/>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="J9" s="16"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="15"/>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
@@ -8501,10 +8509,11 @@
       <c r="G10" s="14"/>
       <c r="H10" s="15"/>
       <c r="I10" s="16"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="15"/>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="J10" s="16"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="15"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
       <c r="C11" s="16"/>
@@ -8514,10 +8523,11 @@
       <c r="G11" s="14"/>
       <c r="H11" s="15"/>
       <c r="I11" s="16"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="15"/>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="J11" s="16"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="15"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="14"/>
       <c r="B12" s="15"/>
       <c r="C12" s="16"/>
@@ -8527,10 +8537,11 @@
       <c r="G12" s="14"/>
       <c r="H12" s="15"/>
       <c r="I12" s="16"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="15"/>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="J12" s="16"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="15"/>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="14"/>
       <c r="B13" s="15"/>
       <c r="C13" s="16"/>
@@ -8540,10 +8551,11 @@
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
       <c r="I13" s="16"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="15"/>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="J13" s="16"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="15"/>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
@@ -8553,10 +8565,11 @@
       <c r="G14" s="14"/>
       <c r="H14" s="15"/>
       <c r="I14" s="16"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="15"/>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="J14" s="16"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="15"/>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
@@ -8566,10 +8579,11 @@
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
       <c r="I15" s="16"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="15"/>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="J15" s="16"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="15"/>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
@@ -8579,10 +8593,11 @@
       <c r="G16" s="14"/>
       <c r="H16" s="15"/>
       <c r="I16" s="16"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="15"/>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="J16" s="16"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="15"/>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
@@ -8592,10 +8607,11 @@
       <c r="G17" s="14"/>
       <c r="H17" s="15"/>
       <c r="I17" s="16"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="15"/>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="J17" s="16"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="15"/>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -8605,14 +8621,15 @@
       <c r="G18" s="14"/>
       <c r="H18" s="15"/>
       <c r="I18" s="16"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="15"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="D4:K4"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="D4:L4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
added extra column to differentiate direct vs indirect cost
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2293 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: abfc717a91ad53c446a151570d5750186c588000
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmart\workspace64bitNew\SEMOSS_2014\export\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahkhalil\newWorkspace\Semoss\export\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="System Overview" sheetId="21" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
   <si>
     <t>Garrison / Theater</t>
   </si>
@@ -369,13 +369,16 @@
     <t>This section displays the current @SYSTEM@ interfaces and how they are affected by DHMSM deployment.</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>Software License Budget</t>
   </si>
   <si>
     <t>Hardware Budget</t>
+  </si>
+  <si>
+    <t>Direct Cost</t>
+  </si>
+  <si>
+    <t>Indirect Cost</t>
   </si>
 </sst>
 </file>
@@ -838,10 +841,22 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -853,6 +868,12 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -862,28 +883,10 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5185,22 +5188,22 @@
     <row r="1" spans="1:18" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:18" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="31"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="35"/>
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
@@ -5229,20 +5232,20 @@
     </row>
     <row r="4" spans="1:18" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
       <c r="N4"/>
       <c r="O4"/>
       <c r="P4"/>
@@ -5283,22 +5286,22 @@
     </row>
     <row r="7" spans="1:18" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="30"/>
+      <c r="D7" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="31"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="35"/>
       <c r="N7"/>
       <c r="O7"/>
       <c r="P7"/>
@@ -5319,20 +5322,20 @@
     </row>
     <row r="9" spans="1:18" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="34"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="40"/>
       <c r="N9"/>
       <c r="O9"/>
       <c r="P9"/>
@@ -5341,30 +5344,30 @@
     </row>
     <row r="10" spans="1:18" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35" t="s">
+      <c r="C10" s="36"/>
+      <c r="D10" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="35" t="s">
+      <c r="E10" s="37"/>
+      <c r="F10" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="36" t="s">
+      <c r="G10" s="36"/>
+      <c r="H10" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="37"/>
-      <c r="J10" s="35" t="s">
+      <c r="I10" s="42"/>
+      <c r="J10" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35" t="s">
+      <c r="K10" s="36"/>
+      <c r="L10" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="35"/>
+      <c r="M10" s="36"/>
       <c r="N10"/>
       <c r="O10"/>
       <c r="P10"/>
@@ -5373,18 +5376,18 @@
     </row>
     <row r="11" spans="1:18" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="39"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="28"/>
       <c r="N11"/>
       <c r="O11"/>
       <c r="P11"/>
@@ -5393,6 +5396,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
@@ -5409,8 +5414,6 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:M7"/>
     <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7684,7 +7687,7 @@
   </sheetPr>
   <dimension ref="A2:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -7828,7 +7831,7 @@
     </row>
     <row r="10" spans="1:10" ht="24" customHeight="1">
       <c r="A10" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="26">
         <v>0</v>
@@ -7836,7 +7839,7 @@
     </row>
     <row r="11" spans="1:10" ht="24" customHeight="1">
       <c r="A11" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="26">
         <v>0</v>
@@ -8384,10 +8387,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8401,13 +8404,13 @@
     <col min="7" max="7" width="16" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" style="1" customWidth="1"/>
     <col min="9" max="10" width="18.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="12" width="25.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" customHeight="1"/>
-    <row r="2" spans="1:12" ht="18" customHeight="1">
+    <row r="1" spans="1:13" ht="18" customHeight="1"/>
+    <row r="2" spans="1:13" ht="18" customHeight="1">
       <c r="A2" s="61" t="s">
         <v>42</v>
       </c>
@@ -8422,8 +8425,9 @@
       <c r="J2" s="61"/>
       <c r="K2" s="61"/>
       <c r="L2" s="61"/>
-    </row>
-    <row r="4" spans="1:12" ht="20.25" customHeight="1">
+      <c r="M2" s="61"/>
+    </row>
+    <row r="4" spans="1:13" ht="20.25" customHeight="1">
       <c r="A4" s="62" t="s">
         <v>3</v>
       </c>
@@ -8439,9 +8443,10 @@
       <c r="I4" s="66"/>
       <c r="J4" s="66"/>
       <c r="K4" s="66"/>
-      <c r="L4" s="67"/>
-    </row>
-    <row r="6" spans="1:12" ht="53.25" customHeight="1">
+      <c r="L4" s="66"/>
+      <c r="M4" s="67"/>
+    </row>
+    <row r="6" spans="1:13" ht="53.25" customHeight="1">
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
@@ -8476,10 +8481,13 @@
         <v>21</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>64</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
@@ -8491,9 +8499,10 @@
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
       <c r="K7" s="14"/>
-      <c r="L7" s="15"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="L7" s="14"/>
+      <c r="M7" s="15"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
       <c r="C8" s="16"/>
@@ -8505,9 +8514,10 @@
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
       <c r="K8" s="14"/>
-      <c r="L8" s="15"/>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="L8" s="14"/>
+      <c r="M8" s="15"/>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
       <c r="C9" s="16"/>
@@ -8519,9 +8529,10 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
       <c r="K9" s="14"/>
-      <c r="L9" s="15"/>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="L9" s="14"/>
+      <c r="M9" s="15"/>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
@@ -8533,9 +8544,10 @@
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
       <c r="K10" s="14"/>
-      <c r="L10" s="15"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="L10" s="14"/>
+      <c r="M10" s="15"/>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
       <c r="C11" s="16"/>
@@ -8547,9 +8559,10 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
       <c r="K11" s="14"/>
-      <c r="L11" s="15"/>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="L11" s="14"/>
+      <c r="M11" s="15"/>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="14"/>
       <c r="B12" s="15"/>
       <c r="C12" s="16"/>
@@ -8561,9 +8574,10 @@
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
       <c r="K12" s="14"/>
-      <c r="L12" s="15"/>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="L12" s="14"/>
+      <c r="M12" s="15"/>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="14"/>
       <c r="B13" s="15"/>
       <c r="C13" s="16"/>
@@ -8575,9 +8589,10 @@
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
       <c r="K13" s="14"/>
-      <c r="L13" s="15"/>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="L13" s="14"/>
+      <c r="M13" s="15"/>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
@@ -8589,9 +8604,10 @@
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
       <c r="K14" s="14"/>
-      <c r="L14" s="15"/>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="L14" s="14"/>
+      <c r="M14" s="15"/>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
@@ -8603,9 +8619,10 @@
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
       <c r="K15" s="14"/>
-      <c r="L15" s="15"/>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="L15" s="14"/>
+      <c r="M15" s="15"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
@@ -8617,9 +8634,10 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
       <c r="K16" s="14"/>
-      <c r="L16" s="15"/>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="L16" s="14"/>
+      <c r="M16" s="15"/>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
@@ -8631,9 +8649,10 @@
       <c r="I17" s="16"/>
       <c r="J17" s="16"/>
       <c r="K17" s="14"/>
-      <c r="L17" s="15"/>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="L17" s="14"/>
+      <c r="M17" s="15"/>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -8645,13 +8664,14 @@
       <c r="I18" s="16"/>
       <c r="J18" s="16"/>
       <c r="K18" s="14"/>
-      <c r="L18" s="15"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="D4:L4"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="D4:M4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
updated template for lpi transition report
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2300 ef391c1c-ee15-45f7-b1d6-dde3d27a2169
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -841,6 +841,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -868,9 +877,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -882,12 +888,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5168,7 +5168,7 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:M7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5188,22 +5188,22 @@
     <row r="1" spans="1:18" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:18" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="33" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="35"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="38"/>
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
@@ -5232,20 +5232,20 @@
     </row>
     <row r="4" spans="1:18" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
       <c r="N4"/>
       <c r="O4"/>
       <c r="P4"/>
@@ -5286,22 +5286,22 @@
     </row>
     <row r="7" spans="1:18" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="33" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="35"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="38"/>
       <c r="N7"/>
       <c r="O7"/>
       <c r="P7"/>
@@ -5322,20 +5322,20 @@
     </row>
     <row r="9" spans="1:18" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="40"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="42"/>
       <c r="N9"/>
       <c r="O9"/>
       <c r="P9"/>
@@ -5344,30 +5344,30 @@
     </row>
     <row r="10" spans="1:18" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36" t="s">
+      <c r="C10" s="27"/>
+      <c r="D10" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="37"/>
-      <c r="F10" s="36" t="s">
+      <c r="E10" s="39"/>
+      <c r="F10" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="41" t="s">
+      <c r="G10" s="27"/>
+      <c r="H10" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="42"/>
-      <c r="J10" s="36" t="s">
+      <c r="I10" s="29"/>
+      <c r="J10" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36" t="s">
+      <c r="K10" s="27"/>
+      <c r="L10" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="36"/>
+      <c r="M10" s="27"/>
       <c r="N10"/>
       <c r="O10"/>
       <c r="P10"/>
@@ -5376,18 +5376,18 @@
     </row>
     <row r="11" spans="1:18" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="28"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="31"/>
       <c r="N11"/>
       <c r="O11"/>
       <c r="P11"/>
@@ -5396,6 +5396,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="B11:C11"/>
@@ -5412,14 +5414,12 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="60" fitToWidth="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup fitToWidth="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;LAHLTA&amp;CSystem Fact Sheets&amp;RPage &amp;P</oddHeader>
+    <oddHeader>&amp;RPage &amp;P</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
@@ -5431,8 +5431,8 @@
   </sheetPr>
   <dimension ref="A2:K114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6548,6 +6548,7 @@
     <mergeCell ref="A3:G3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="89" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -6559,8 +6560,8 @@
   </sheetPr>
   <dimension ref="A2:K114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7676,6 +7677,7 @@
     <mergeCell ref="C42:G43"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="89" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -7687,8 +7689,8 @@
   </sheetPr>
   <dimension ref="A2:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7851,6 +7853,7 @@
     <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -7862,8 +7865,8 @@
   </sheetPr>
   <dimension ref="A2:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8037,6 +8040,7 @@
     <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -8046,43 +8050,42 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A2:C30"/>
+  <dimension ref="A2:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="45.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="44.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="58.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="18">
+    <row r="2" spans="1:2" ht="18">
       <c r="A2" s="61" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="61"/>
     </row>
-    <row r="3" spans="1:3" ht="18">
+    <row r="3" spans="1:2" ht="18">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
     </row>
-    <row r="4" spans="1:3" ht="50.25" customHeight="1">
+    <row r="4" spans="1:2" ht="50.25" customHeight="1">
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C4"/>
-    </row>
-    <row r="5" spans="1:3">
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:2">
       <c r="A6" s="17" t="s">
         <v>9</v>
       </c>
@@ -8090,43 +8093,43 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:2">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:2">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:2">
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:2">
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:2">
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:2">
       <c r="A12" s="14"/>
       <c r="B12" s="15"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:2">
       <c r="A13" s="14"/>
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:2">
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:2">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:2">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
     </row>
@@ -8191,6 +8194,7 @@
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="99" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -8202,15 +8206,15 @@
   </sheetPr>
   <dimension ref="A2:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="26.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="71.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -8377,7 +8381,7 @@
     <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="69" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -8389,8 +8393,8 @@
   </sheetPr>
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8398,14 +8402,16 @@
     <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="1" customWidth="1"/>
-    <col min="9" max="10" width="18.28515625" style="1" customWidth="1"/>
-    <col min="11" max="12" width="25.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16" style="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -8674,6 +8680,7 @@
     <mergeCell ref="D4:M4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="48" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed header from lpi report template
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2301 ef391c1c-ee15-45f7-b1d6-dde3d27a2169
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727"/>
   </bookViews>
   <sheets>
     <sheet name="System Overview" sheetId="21" r:id="rId1"/>
@@ -841,6 +841,24 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -868,26 +886,8 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5167,7 +5167,7 @@
   </sheetPr>
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -5188,22 +5188,22 @@
     <row r="1" spans="1:18" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:18" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="36" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="38"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="29"/>
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
@@ -5232,20 +5232,20 @@
     </row>
     <row r="4" spans="1:18" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
       <c r="N4"/>
       <c r="O4"/>
       <c r="P4"/>
@@ -5286,22 +5286,22 @@
     </row>
     <row r="7" spans="1:18" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="36" t="s">
+      <c r="C7" s="39"/>
+      <c r="D7" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="38"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="29"/>
       <c r="N7"/>
       <c r="O7"/>
       <c r="P7"/>
@@ -5322,20 +5322,20 @@
     </row>
     <row r="9" spans="1:18" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="42"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="32"/>
       <c r="N9"/>
       <c r="O9"/>
       <c r="P9"/>
@@ -5344,30 +5344,30 @@
     </row>
     <row r="10" spans="1:18" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27" t="s">
+      <c r="C10" s="33"/>
+      <c r="D10" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="27" t="s">
+      <c r="E10" s="42"/>
+      <c r="F10" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28" t="s">
+      <c r="G10" s="33"/>
+      <c r="H10" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="29"/>
-      <c r="J10" s="27" t="s">
+      <c r="I10" s="35"/>
+      <c r="J10" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27" t="s">
+      <c r="K10" s="33"/>
+      <c r="L10" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="27"/>
+      <c r="M10" s="33"/>
       <c r="N10"/>
       <c r="O10"/>
       <c r="P10"/>
@@ -5376,18 +5376,18 @@
     </row>
     <row r="11" spans="1:18" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="31"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="37"/>
       <c r="N11"/>
       <c r="O11"/>
       <c r="P11"/>
@@ -5396,11 +5396,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -5414,13 +5409,15 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToWidth="0" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;RPage &amp;P</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -8393,7 +8390,7 @@
   </sheetPr>
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added freeze pane during printing to template
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2302 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: c3830c7925e96b7251c0bae8340f306b4b588397
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="System Overview" sheetId="21" r:id="rId1"/>
@@ -64,7 +64,12 @@
     <definedName name="ODS_SUM">'[2]POM 2 Enabler - FY12'!$M$102</definedName>
     <definedName name="Portal_ROI">[2]BOM!$N$46</definedName>
     <definedName name="Portal_SUM">'[2]POM 2 Enabler - FY12'!$N$102</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Software Lifecycles'!$A$8:$G$8</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'System Overview'!$A$2:$Q$11</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">'Data Provenance'!$6:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="6">'DHMSM Data Requirements'!$6:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">'System Data'!$6:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="7">'System Interfaces'!$6:$6</definedName>
     <definedName name="Priority3">[4]Data1!$B$4:$B$6</definedName>
     <definedName name="ProcContractMonths">'[2]New Timeline'!$A$22</definedName>
     <definedName name="RangeBLU">[5]BLUBackEnd!$G$5:$G$49</definedName>
@@ -5167,7 +5172,7 @@
   </sheetPr>
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -5429,7 +5434,7 @@
   <dimension ref="A2:K114"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:G8"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7863,7 +7868,7 @@
   <dimension ref="A2:C30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8050,7 +8055,7 @@
   <dimension ref="A2:B30"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="A6:B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8204,7 +8209,7 @@
   <dimension ref="A2:C30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C6"/>
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8390,8 +8395,8 @@
   </sheetPr>
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
edited format for lpi transition template
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2303 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 319afb75464458867e6521b4bd0f8bbeb4a54626
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="System Overview" sheetId="21" r:id="rId1"/>
@@ -64,10 +64,11 @@
     <definedName name="ODS_SUM">'[2]POM 2 Enabler - FY12'!$M$102</definedName>
     <definedName name="Portal_ROI">[2]BOM!$N$46</definedName>
     <definedName name="Portal_SUM">'[2]POM 2 Enabler - FY12'!$N$102</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Software Lifecycles'!$A$8:$G$8</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'System Overview'!$A$2:$Q$11</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="5">'Data Provenance'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">'DHMSM Data Requirements'!$6:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Hardware Lifecycles'!$8:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Software Lifecycles'!$8:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'System Data'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="7">'System Interfaces'!$6:$6</definedName>
     <definedName name="Priority3">[4]Data1!$B$4:$B$6</definedName>
@@ -5433,8 +5434,8 @@
   </sheetPr>
   <dimension ref="A2:K114"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6563,7 +6564,7 @@
   <dimension ref="A2:K114"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:G8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8395,7 +8396,7 @@
   </sheetPr>
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated formatting for lpi report
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2314 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: cc6734d0bb0d1ee6627d08c30cdc975df92ba9c2
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="System Overview" sheetId="21" r:id="rId1"/>
@@ -116,15 +116,6 @@
     <t>MHS-Specific</t>
   </si>
   <si>
-    <t>Transaction Count</t>
-  </si>
-  <si>
-    <t>ATO Date</t>
-  </si>
-  <si>
-    <t>End of Support</t>
-  </si>
-  <si>
     <t>Data Object</t>
   </si>
   <si>
@@ -132,9 +123,6 @@
   </si>
   <si>
     <t>Capability</t>
-  </si>
-  <si>
-    <t>Comments</t>
   </si>
   <si>
     <t>Data Provenance</t>
@@ -168,9 +156,6 @@
   </si>
   <si>
     <t>Software Version</t>
-  </si>
-  <si>
-    <t>Support Date</t>
   </si>
   <si>
     <t>Unit Cost</t>
@@ -386,11 +371,29 @@
   <si>
     <t>Indirect Cost</t>
   </si>
+  <si>
+    <t>Average Daily Transaction Count</t>
+  </si>
+  <si>
+    <t>ATO Date Received</t>
+  </si>
+  <si>
+    <t>Scheduled End of Support</t>
+  </si>
+  <si>
+    <t>End of Support Date</t>
+  </si>
+  <si>
+    <t>System Source of Record Business Rule</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="23">
     <font>
       <sz val="11"/>
@@ -725,7 +728,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -784,8 +787,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -847,27 +851,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -892,8 +875,29 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -970,10 +974,19 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="50">
     <cellStyle name="%" xfId="2"/>
     <cellStyle name="% 2" xfId="3"/>
+    <cellStyle name="Currency" xfId="49" builtinId="4"/>
     <cellStyle name="Hyperlink 2" xfId="4"/>
     <cellStyle name="Hyperlink 2 2" xfId="5"/>
     <cellStyle name="Hyperlink 2 2 2" xfId="6"/>
@@ -5173,8 +5186,8 @@
   </sheetPr>
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5194,22 +5207,22 @@
     <row r="1" spans="1:18" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:18" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="29"/>
+      <c r="B2" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="37"/>
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
@@ -5238,20 +5251,20 @@
     </row>
     <row r="4" spans="1:18" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
+      <c r="B4" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
       <c r="N4"/>
       <c r="O4"/>
       <c r="P4"/>
@@ -5292,22 +5305,22 @@
     </row>
     <row r="7" spans="1:18" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="29"/>
+      <c r="B7" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="32"/>
+      <c r="D7" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="37"/>
       <c r="N7"/>
       <c r="O7"/>
       <c r="P7"/>
@@ -5328,20 +5341,20 @@
     </row>
     <row r="9" spans="1:18" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="32"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="42"/>
       <c r="N9"/>
       <c r="O9"/>
       <c r="P9"/>
@@ -5350,30 +5363,30 @@
     </row>
     <row r="10" spans="1:18" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33" t="s">
+      <c r="C10" s="38"/>
+      <c r="D10" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="35"/>
-      <c r="J10" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33" t="s">
+      <c r="E10" s="39"/>
+      <c r="F10" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="38"/>
+      <c r="H10" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="28"/>
+      <c r="J10" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="33"/>
+      <c r="M10" s="38"/>
       <c r="N10"/>
       <c r="O10"/>
       <c r="P10"/>
@@ -5382,18 +5395,18 @@
     </row>
     <row r="11" spans="1:18" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="37"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="30"/>
       <c r="N11"/>
       <c r="O11"/>
       <c r="P11"/>
@@ -5402,6 +5415,10 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -5416,10 +5433,6 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5434,8 +5447,8 @@
   </sheetPr>
   <dimension ref="A2:K114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5452,7 +5465,7 @@
   <sheetData>
     <row r="2" spans="1:11" ht="18" customHeight="1">
       <c r="A2" s="53" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B2" s="53"/>
       <c r="C2" s="53"/>
@@ -5467,7 +5480,7 @@
     </row>
     <row r="3" spans="1:11" ht="18" customHeight="1">
       <c r="A3" s="54" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B3" s="54"/>
       <c r="C3" s="54"/>
@@ -5482,11 +5495,11 @@
     </row>
     <row r="5" spans="1:11" ht="18.75" customHeight="1">
       <c r="A5" s="43" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B5" s="44"/>
       <c r="C5" s="47" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D5" s="48"/>
       <c r="E5" s="48"/>
@@ -5512,25 +5525,25 @@
     </row>
     <row r="8" spans="1:11" ht="26.25">
       <c r="A8" s="17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F8" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="17" t="s">
         <v>27</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>32</v>
       </c>
       <c r="H8"/>
       <c r="I8"/>
@@ -5875,11 +5888,11 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="43" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B42" s="44"/>
       <c r="C42" s="47" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D42" s="48"/>
       <c r="E42" s="48"/>
@@ -5897,25 +5910,25 @@
     </row>
     <row r="45" spans="1:7" ht="25.5">
       <c r="A45" s="17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F45" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" s="17" t="s">
         <v>27</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -6208,11 +6221,11 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="43" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B79" s="44"/>
       <c r="C79" s="47" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D79" s="48"/>
       <c r="E79" s="48"/>
@@ -6230,25 +6243,25 @@
     </row>
     <row r="82" spans="1:7" ht="25.5">
       <c r="A82" s="17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D82" s="17" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E82" s="17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F82" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G82" s="17" t="s">
         <v>27</v>
-      </c>
-      <c r="G82" s="17" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -6563,8 +6576,8 @@
   </sheetPr>
   <dimension ref="A2:K114"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6581,7 +6594,7 @@
   <sheetData>
     <row r="2" spans="1:11" ht="18" customHeight="1">
       <c r="A2" s="55" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B2" s="56"/>
       <c r="C2" s="56"/>
@@ -6611,11 +6624,11 @@
     </row>
     <row r="5" spans="1:11" ht="18.75" customHeight="1">
       <c r="A5" s="43" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B5" s="44"/>
       <c r="C5" s="47" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D5" s="48"/>
       <c r="E5" s="48"/>
@@ -6641,25 +6654,25 @@
     </row>
     <row r="8" spans="1:11" ht="26.25">
       <c r="A8" s="17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H8"/>
       <c r="I8"/>
@@ -7004,11 +7017,11 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="43" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B42" s="44"/>
       <c r="C42" s="47" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D42" s="48"/>
       <c r="E42" s="48"/>
@@ -7026,25 +7039,25 @@
     </row>
     <row r="45" spans="1:7" ht="25.5">
       <c r="A45" s="17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -7337,11 +7350,11 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="43" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B79" s="44"/>
       <c r="C79" s="47" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D79" s="48"/>
       <c r="E79" s="48"/>
@@ -7359,25 +7372,25 @@
     </row>
     <row r="82" spans="1:7" ht="25.5">
       <c r="A82" s="17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D82" s="17" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E82" s="17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G82" s="17" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -7705,7 +7718,7 @@
   <sheetData>
     <row r="2" spans="1:10" ht="18" customHeight="1">
       <c r="A2" s="61" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B2" s="61"/>
       <c r="C2" s="61"/>
@@ -7726,7 +7739,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C4" s="59"/>
       <c r="D4" s="59"/>
@@ -7767,12 +7780,12 @@
         <v>2022</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="24" customHeight="1">
       <c r="A7" s="25" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B7" s="26">
         <v>0</v>
@@ -7804,7 +7817,7 @@
     </row>
     <row r="8" spans="1:10" ht="24" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B8" s="26">
         <v>0</v>
@@ -7836,7 +7849,7 @@
     </row>
     <row r="10" spans="1:10" ht="24" customHeight="1">
       <c r="A10" s="25" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B10" s="26">
         <v>0</v>
@@ -7844,7 +7857,7 @@
     </row>
     <row r="11" spans="1:10" ht="24" customHeight="1">
       <c r="A11" s="25" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B11" s="26">
         <v>0</v>
@@ -7882,7 +7895,7 @@
   <sheetData>
     <row r="2" spans="1:3" ht="18">
       <c r="A2" s="61" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" s="61"/>
       <c r="C2" s="61"/>
@@ -7897,7 +7910,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C4" s="60"/>
     </row>
@@ -7908,13 +7921,13 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -8068,7 +8081,7 @@
   <sheetData>
     <row r="2" spans="1:2" ht="18">
       <c r="A2" s="61" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B2" s="61"/>
     </row>
@@ -8081,7 +8094,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -8090,10 +8103,10 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -8210,7 +8223,7 @@
   <dimension ref="A2:C30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8223,7 +8236,7 @@
   <sheetData>
     <row r="2" spans="1:3" ht="18">
       <c r="A2" s="61" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B2" s="61"/>
       <c r="C2" s="61"/>
@@ -8238,7 +8251,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C4" s="60"/>
     </row>
@@ -8249,13 +8262,13 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -8396,8 +8409,8 @@
   </sheetPr>
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8413,15 +8426,15 @@
     <col min="9" max="9" width="17.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="24" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15" style="68" customWidth="1"/>
+    <col min="13" max="13" width="16" style="68" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1"/>
     <row r="2" spans="1:13" ht="18" customHeight="1">
       <c r="A2" s="61" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B2" s="61"/>
       <c r="C2" s="61"/>
@@ -8443,7 +8456,7 @@
       <c r="B4" s="63"/>
       <c r="C4" s="64"/>
       <c r="D4" s="65" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E4" s="66"/>
       <c r="F4" s="66"/>
@@ -8460,40 +8473,40 @@
         <v>2</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="17" t="s">
+      <c r="I6" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="L6" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>65</v>
+      <c r="L6" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="M6" s="69" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -8508,8 +8521,8 @@
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
       <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="15"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="71"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="14"/>
@@ -8523,8 +8536,8 @@
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
       <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="15"/>
+      <c r="L8" s="70"/>
+      <c r="M8" s="71"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="14"/>
@@ -8538,8 +8551,8 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
       <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="15"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="71"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="14"/>
@@ -8553,8 +8566,8 @@
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
       <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="15"/>
+      <c r="L10" s="70"/>
+      <c r="M10" s="71"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="14"/>
@@ -8568,8 +8581,8 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
       <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="15"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="71"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="14"/>
@@ -8583,8 +8596,8 @@
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
       <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="15"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="71"/>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="14"/>
@@ -8598,8 +8611,8 @@
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
       <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="15"/>
+      <c r="L13" s="70"/>
+      <c r="M13" s="71"/>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="14"/>
@@ -8613,8 +8626,8 @@
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
       <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="15"/>
+      <c r="L14" s="70"/>
+      <c r="M14" s="71"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="14"/>
@@ -8628,8 +8641,8 @@
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
       <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="15"/>
+      <c r="L15" s="70"/>
+      <c r="M15" s="71"/>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="14"/>
@@ -8643,8 +8656,8 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
       <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="15"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="71"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="14"/>
@@ -8658,8 +8671,8 @@
       <c r="I17" s="16"/>
       <c r="J17" s="16"/>
       <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="15"/>
+      <c r="L17" s="70"/>
+      <c r="M17" s="71"/>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="14"/>
@@ -8673,8 +8686,8 @@
       <c r="I18" s="16"/>
       <c r="J18" s="16"/>
       <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="15"/>
+      <c r="L18" s="70"/>
+      <c r="M18" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
updated lpi report to account for accounting
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2322 ef391c1c-ee15-45f7-b1d6-dde3d27a2169
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahkhalil\newWorkspace\Semoss\export\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmart\workspace64bitNew\SEMOSS_2014\export\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="System Overview" sheetId="21" r:id="rId1"/>
@@ -64,11 +64,11 @@
     <definedName name="ODS_SUM">'[2]POM 2 Enabler - FY12'!$M$102</definedName>
     <definedName name="Portal_ROI">[2]BOM!$N$46</definedName>
     <definedName name="Portal_SUM">'[2]POM 2 Enabler - FY12'!$N$102</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'System Overview'!$A$2:$Q$11</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'System Overview'!$A$2:$M$11</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="5">'Data Provenance'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">'DHMSM Data Requirements'!$6:$6</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Hardware Lifecycles'!$8:$8</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Software Lifecycles'!$8:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Hardware Lifecycles'!$7:$7</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Software Lifecycles'!$7:$7</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'System Data'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="7">'System Interfaces'!$6:$6</definedName>
     <definedName name="Priority3">[4]Data1!$B$4:$B$6</definedName>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
   <si>
     <t>Garrison / Theater</t>
   </si>
@@ -170,12 +170,6 @@
     <t>Current State</t>
   </si>
   <si>
-    <t>IOC</t>
-  </si>
-  <si>
-    <t>FOC</t>
-  </si>
-  <si>
     <t>Hardware Lifecycles</t>
   </si>
   <si>
@@ -210,90 +204,6 @@
   </si>
   <si>
     <t>System Interfaces</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Software life cycle at  the start of IOC </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(expected @DATE@)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Hardware life cycle at  the start of IOC </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(expected @DATE@)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Software life cycle at IOC</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (expected @DATE@)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Software life cycle at FOC </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(expected @DATE@)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Hardware life cycle at IOC</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (expected @DATE@)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Hardware life cycle at FOC </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(expected @DATE@)</t>
-    </r>
   </si>
   <si>
     <t>This section displays the data objects that @SYSTEM@ provides and consumes.</t>
@@ -386,15 +296,47 @@
   <si>
     <t>System Source of Record Business Rule</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Software life cycle at the start of IOC </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(expected @DATE@)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hardware life cycle at the start of IOC </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(expected @DATE@)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,13 +402,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -547,6 +482,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -592,7 +539,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -620,17 +567,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -786,171 +722,177 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="48" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="48" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="48" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="48"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="48" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="48"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="48" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="48" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="48" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="48" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="48" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="48" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="22" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="23" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="48" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -959,11 +901,8 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -971,17 +910,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="%" xfId="2"/>
@@ -5184,10 +5112,10 @@
     <tabColor theme="4" tint="-6.1037018951994385E-5"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="D2" sqref="D2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5200,78 +5128,62 @@
     <col min="7" max="7" width="9" style="6" customWidth="1"/>
     <col min="8" max="10" width="7.5703125" style="6" customWidth="1"/>
     <col min="11" max="13" width="7.42578125" style="6" customWidth="1"/>
-    <col min="14" max="17" width="8" style="6" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="6"/>
+    <col min="14" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="7.5" customHeight="1"/>
-    <row r="2" spans="1:18" s="4" customFormat="1" ht="250.5" customHeight="1">
+    <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="37"/>
-      <c r="N2"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
+      <c r="B2" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="43"/>
     </row>
-    <row r="3" spans="1:18" s="24" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
+    <row r="3" spans="1:13" s="21" customFormat="1" ht="7.5" customHeight="1">
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
     </row>
-    <row r="4" spans="1:18" ht="32.25" customHeight="1">
+    <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
+      <c r="B4" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
     </row>
-    <row r="5" spans="1:18" ht="7.5" customHeight="1">
+    <row r="5" spans="1:13" ht="7.5" customHeight="1">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -5285,133 +5197,98 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
-      <c r="R5"/>
     </row>
-    <row r="6" spans="1:18" ht="0.75" customHeight="1">
+    <row r="6" spans="1:13" ht="0.75" customHeight="1">
       <c r="A6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="10"/>
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
     </row>
-    <row r="7" spans="1:18" s="4" customFormat="1" ht="168.75" customHeight="1">
+    <row r="7" spans="1:13" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="37"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
+      <c r="B7" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="D7" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="43"/>
     </row>
-    <row r="8" spans="1:18" ht="8.25" customHeight="1">
+    <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
-      <c r="Q8"/>
-      <c r="R8"/>
     </row>
-    <row r="9" spans="1:18" s="8" customFormat="1" ht="18" customHeight="1">
+    <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="42"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9"/>
-      <c r="R9"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="48"/>
     </row>
-    <row r="10" spans="1:18" s="8" customFormat="1" ht="28.5" customHeight="1">
+    <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38" t="s">
+      <c r="C10" s="44"/>
+      <c r="D10" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="38"/>
-      <c r="H10" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="I10" s="28"/>
-      <c r="J10" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38" t="s">
+      <c r="E10" s="45"/>
+      <c r="F10" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="44"/>
+      <c r="H10" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="34"/>
+      <c r="J10" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="38"/>
-      <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
+      <c r="M10" s="44"/>
     </row>
-    <row r="11" spans="1:18" ht="42.75" customHeight="1">
+    <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="30"/>
-      <c r="N11"/>
-      <c r="O11"/>
-      <c r="P11"/>
-      <c r="Q11"/>
-      <c r="R11"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -5445,1122 +5322,116 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A2:K114"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="18" customHeight="1">
-      <c r="A2" s="53" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18" customHeight="1">
+      <c r="A2" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
     </row>
-    <row r="3" spans="1:11" ht="18" customHeight="1">
-      <c r="A3" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
+    <row r="3" spans="1:7" ht="18" customHeight="1">
+      <c r="A3" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
     </row>
-    <row r="5" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A5" s="43" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A5" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="49"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="52"/>
     </row>
-    <row r="6" spans="1:11" ht="30.75" customHeight="1">
-      <c r="A6" s="45"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="52"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" ht="26.25">
-      <c r="A8" s="17" t="s">
+    <row r="7" spans="1:7" ht="25.5">
+      <c r="A7" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="17" t="s">
+      <c r="B7" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E7" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F7" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
+      <c r="G7" s="22" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" ht="15">
-      <c r="A9" s="16"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
+    <row r="8" spans="1:7">
+      <c r="A8" s="25"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="31"/>
     </row>
-    <row r="10" spans="1:11" ht="15">
-      <c r="A10" s="16"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16"/>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-      <c r="K10"/>
-    </row>
-    <row r="11" spans="1:11" ht="15">
-      <c r="A11" s="16"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="16"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-    </row>
-    <row r="12" spans="1:11" ht="15">
-      <c r="A12" s="16"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-    </row>
-    <row r="13" spans="1:11" ht="15">
-      <c r="A13" s="16"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-    </row>
-    <row r="14" spans="1:11" ht="15">
-      <c r="A14" s="16"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="16"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-      <c r="K14"/>
-    </row>
-    <row r="15" spans="1:11" ht="15">
-      <c r="A15" s="16"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-    </row>
-    <row r="16" spans="1:11" ht="15">
-      <c r="A16" s="16"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-    </row>
-    <row r="17" spans="1:11" ht="15">
-      <c r="A17" s="16"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="16"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
-      <c r="K17"/>
-    </row>
-    <row r="18" spans="1:11" ht="15">
-      <c r="A18" s="16"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
-      <c r="K18"/>
-    </row>
-    <row r="19" spans="1:11" ht="15">
-      <c r="A19" s="16"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="16"/>
-      <c r="H19"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-    </row>
-    <row r="20" spans="1:11" ht="15">
-      <c r="A20" s="16"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="16"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="16"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="16"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="16"/>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="16"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="16"/>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="16"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="16"/>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="16"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="16"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="16"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="16"/>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="16"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="16"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="16"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="16"/>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="16"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="16"/>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="16"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="16"/>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="16"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="16"/>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="16"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="16"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="16"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="16"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="16"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="16"/>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="16"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="16"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="16"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="16"/>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="16"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="16"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="16"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="16"/>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="16"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="16"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="16"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="16"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" s="44"/>
-      <c r="C42" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="49"/>
-    </row>
-    <row r="43" spans="1:7" ht="32.25" customHeight="1">
-      <c r="A43" s="45"/>
-      <c r="B43" s="46"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="51"/>
-      <c r="F43" s="51"/>
-      <c r="G43" s="52"/>
-    </row>
-    <row r="45" spans="1:7" ht="25.5">
-      <c r="A45" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="16"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="16"/>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="16"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="16"/>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="16"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="16"/>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="16"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="16"/>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="16"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="16"/>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="16"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="16"/>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="16"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="16"/>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" s="16"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="16"/>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="16"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="16"/>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" s="16"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="16"/>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" s="16"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="16"/>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57" s="16"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="15"/>
-      <c r="G57" s="16"/>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="16"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="16"/>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="16"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="16"/>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="16"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="16"/>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="16"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="15"/>
-      <c r="G61" s="16"/>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="16"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="15"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="15"/>
-      <c r="G62" s="16"/>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="16"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="15"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="16"/>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="16"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="15"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="15"/>
-      <c r="G64" s="16"/>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="16"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="16"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="15"/>
-      <c r="G65" s="16"/>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="16"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="16"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="16"/>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" s="16"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="15"/>
-      <c r="G67" s="16"/>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="16"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="16"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="15"/>
-      <c r="G68" s="16"/>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="16"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="15"/>
-      <c r="D69" s="16"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="15"/>
-      <c r="G69" s="16"/>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" s="16"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="15"/>
-      <c r="D70" s="16"/>
-      <c r="E70" s="14"/>
-      <c r="F70" s="15"/>
-      <c r="G70" s="16"/>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" s="16"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="15"/>
-      <c r="D71" s="16"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="15"/>
-      <c r="G71" s="16"/>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="16"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="15"/>
-      <c r="D72" s="16"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="15"/>
-      <c r="G72" s="16"/>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="A73" s="16"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="15"/>
-      <c r="D73" s="16"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="15"/>
-      <c r="G73" s="16"/>
-    </row>
-    <row r="74" spans="1:7">
-      <c r="A74" s="16"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="16"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="15"/>
-      <c r="G74" s="16"/>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="A75" s="16"/>
-      <c r="B75" s="14"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="16"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="15"/>
-      <c r="G75" s="16"/>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" s="16"/>
-      <c r="B76" s="14"/>
-      <c r="C76" s="15"/>
-      <c r="D76" s="16"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="15"/>
-      <c r="G76" s="16"/>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="A77" s="16"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="15"/>
-      <c r="D77" s="16"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="15"/>
-      <c r="G77" s="16"/>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="A79" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="B79" s="44"/>
-      <c r="C79" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="D79" s="48"/>
-      <c r="E79" s="48"/>
-      <c r="F79" s="48"/>
-      <c r="G79" s="49"/>
-    </row>
-    <row r="80" spans="1:7" ht="31.5" customHeight="1">
-      <c r="A80" s="45"/>
-      <c r="B80" s="46"/>
-      <c r="C80" s="50"/>
-      <c r="D80" s="51"/>
-      <c r="E80" s="51"/>
-      <c r="F80" s="51"/>
-      <c r="G80" s="52"/>
-    </row>
-    <row r="82" spans="1:7" ht="25.5">
-      <c r="A82" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B82" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C82" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D82" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E82" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F82" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G82" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7">
-      <c r="A83" s="16"/>
-      <c r="B83" s="14"/>
-      <c r="C83" s="15"/>
-      <c r="D83" s="16"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="15"/>
-      <c r="G83" s="16"/>
-    </row>
-    <row r="84" spans="1:7">
-      <c r="A84" s="16"/>
-      <c r="B84" s="14"/>
-      <c r="C84" s="15"/>
-      <c r="D84" s="16"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="15"/>
-      <c r="G84" s="16"/>
-    </row>
-    <row r="85" spans="1:7">
-      <c r="A85" s="16"/>
-      <c r="B85" s="14"/>
-      <c r="C85" s="15"/>
-      <c r="D85" s="16"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="15"/>
-      <c r="G85" s="16"/>
-    </row>
-    <row r="86" spans="1:7">
-      <c r="A86" s="16"/>
-      <c r="B86" s="14"/>
-      <c r="C86" s="15"/>
-      <c r="D86" s="16"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="15"/>
-      <c r="G86" s="16"/>
-    </row>
-    <row r="87" spans="1:7">
-      <c r="A87" s="16"/>
-      <c r="B87" s="14"/>
-      <c r="C87" s="15"/>
-      <c r="D87" s="16"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="15"/>
-      <c r="G87" s="16"/>
-    </row>
-    <row r="88" spans="1:7">
-      <c r="A88" s="16"/>
-      <c r="B88" s="14"/>
-      <c r="C88" s="15"/>
-      <c r="D88" s="16"/>
-      <c r="E88" s="14"/>
-      <c r="F88" s="15"/>
-      <c r="G88" s="16"/>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="A89" s="16"/>
-      <c r="B89" s="14"/>
-      <c r="C89" s="15"/>
-      <c r="D89" s="16"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="15"/>
-      <c r="G89" s="16"/>
-    </row>
-    <row r="90" spans="1:7">
-      <c r="A90" s="16"/>
-      <c r="B90" s="14"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="16"/>
-      <c r="E90" s="14"/>
-      <c r="F90" s="15"/>
-      <c r="G90" s="16"/>
-    </row>
-    <row r="91" spans="1:7">
-      <c r="A91" s="16"/>
-      <c r="B91" s="14"/>
-      <c r="C91" s="15"/>
-      <c r="D91" s="16"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="15"/>
-      <c r="G91" s="16"/>
-    </row>
-    <row r="92" spans="1:7">
-      <c r="A92" s="16"/>
-      <c r="B92" s="14"/>
-      <c r="C92" s="15"/>
-      <c r="D92" s="16"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="15"/>
-      <c r="G92" s="16"/>
-    </row>
-    <row r="93" spans="1:7">
-      <c r="A93" s="16"/>
-      <c r="B93" s="14"/>
-      <c r="C93" s="15"/>
-      <c r="D93" s="16"/>
-      <c r="E93" s="14"/>
-      <c r="F93" s="15"/>
-      <c r="G93" s="16"/>
-    </row>
-    <row r="94" spans="1:7">
-      <c r="A94" s="16"/>
-      <c r="B94" s="14"/>
-      <c r="C94" s="15"/>
-      <c r="D94" s="16"/>
-      <c r="E94" s="14"/>
-      <c r="F94" s="15"/>
-      <c r="G94" s="16"/>
-    </row>
-    <row r="95" spans="1:7">
-      <c r="A95" s="16"/>
-      <c r="B95" s="14"/>
-      <c r="C95" s="15"/>
-      <c r="D95" s="16"/>
-      <c r="E95" s="14"/>
-      <c r="F95" s="15"/>
-      <c r="G95" s="16"/>
-    </row>
-    <row r="96" spans="1:7">
-      <c r="A96" s="16"/>
-      <c r="B96" s="14"/>
-      <c r="C96" s="15"/>
-      <c r="D96" s="16"/>
-      <c r="E96" s="14"/>
-      <c r="F96" s="15"/>
-      <c r="G96" s="16"/>
-    </row>
-    <row r="97" spans="1:7">
-      <c r="A97" s="16"/>
-      <c r="B97" s="14"/>
-      <c r="C97" s="15"/>
-      <c r="D97" s="16"/>
-      <c r="E97" s="14"/>
-      <c r="F97" s="15"/>
-      <c r="G97" s="16"/>
-    </row>
-    <row r="98" spans="1:7">
-      <c r="A98" s="16"/>
-      <c r="B98" s="14"/>
-      <c r="C98" s="15"/>
-      <c r="D98" s="16"/>
-      <c r="E98" s="14"/>
-      <c r="F98" s="15"/>
-      <c r="G98" s="16"/>
-    </row>
-    <row r="99" spans="1:7">
-      <c r="A99" s="16"/>
-      <c r="B99" s="14"/>
-      <c r="C99" s="15"/>
-      <c r="D99" s="16"/>
-      <c r="E99" s="14"/>
-      <c r="F99" s="15"/>
-      <c r="G99" s="16"/>
-    </row>
-    <row r="100" spans="1:7">
-      <c r="A100" s="16"/>
-      <c r="B100" s="14"/>
-      <c r="C100" s="15"/>
-      <c r="D100" s="16"/>
-      <c r="E100" s="14"/>
-      <c r="F100" s="15"/>
-      <c r="G100" s="16"/>
-    </row>
-    <row r="101" spans="1:7">
-      <c r="A101" s="16"/>
-      <c r="B101" s="14"/>
-      <c r="C101" s="15"/>
-      <c r="D101" s="16"/>
-      <c r="E101" s="14"/>
-      <c r="F101" s="15"/>
-      <c r="G101" s="16"/>
-    </row>
-    <row r="102" spans="1:7">
-      <c r="A102" s="16"/>
-      <c r="B102" s="14"/>
-      <c r="C102" s="15"/>
-      <c r="D102" s="16"/>
-      <c r="E102" s="14"/>
-      <c r="F102" s="15"/>
-      <c r="G102" s="16"/>
-    </row>
-    <row r="103" spans="1:7">
-      <c r="A103" s="16"/>
-      <c r="B103" s="14"/>
-      <c r="C103" s="15"/>
-      <c r="D103" s="16"/>
-      <c r="E103" s="14"/>
-      <c r="F103" s="15"/>
-      <c r="G103" s="16"/>
-    </row>
-    <row r="104" spans="1:7">
-      <c r="A104" s="16"/>
-      <c r="B104" s="14"/>
-      <c r="C104" s="15"/>
-      <c r="D104" s="16"/>
-      <c r="E104" s="14"/>
-      <c r="F104" s="15"/>
-      <c r="G104" s="16"/>
-    </row>
-    <row r="105" spans="1:7">
-      <c r="A105" s="16"/>
-      <c r="B105" s="14"/>
-      <c r="C105" s="15"/>
-      <c r="D105" s="16"/>
-      <c r="E105" s="14"/>
-      <c r="F105" s="15"/>
-      <c r="G105" s="16"/>
-    </row>
-    <row r="106" spans="1:7">
-      <c r="A106" s="16"/>
-      <c r="B106" s="14"/>
-      <c r="C106" s="15"/>
-      <c r="D106" s="16"/>
-      <c r="E106" s="14"/>
-      <c r="F106" s="15"/>
-      <c r="G106" s="16"/>
-    </row>
-    <row r="107" spans="1:7">
-      <c r="A107" s="16"/>
-      <c r="B107" s="14"/>
-      <c r="C107" s="15"/>
-      <c r="D107" s="16"/>
-      <c r="E107" s="14"/>
-      <c r="F107" s="15"/>
-      <c r="G107" s="16"/>
-    </row>
-    <row r="108" spans="1:7">
-      <c r="A108" s="16"/>
-      <c r="B108" s="14"/>
-      <c r="C108" s="15"/>
-      <c r="D108" s="16"/>
-      <c r="E108" s="14"/>
-      <c r="F108" s="15"/>
-      <c r="G108" s="16"/>
-    </row>
-    <row r="109" spans="1:7">
-      <c r="A109" s="16"/>
-      <c r="B109" s="14"/>
-      <c r="C109" s="15"/>
-      <c r="D109" s="16"/>
-      <c r="E109" s="14"/>
-      <c r="F109" s="15"/>
-      <c r="G109" s="16"/>
-    </row>
-    <row r="110" spans="1:7">
-      <c r="A110" s="16"/>
-      <c r="B110" s="14"/>
-      <c r="C110" s="15"/>
-      <c r="D110" s="16"/>
-      <c r="E110" s="14"/>
-      <c r="F110" s="15"/>
-      <c r="G110" s="16"/>
-    </row>
-    <row r="111" spans="1:7">
-      <c r="A111" s="16"/>
-      <c r="B111" s="14"/>
-      <c r="C111" s="15"/>
-      <c r="D111" s="16"/>
-      <c r="E111" s="14"/>
-      <c r="F111" s="15"/>
-      <c r="G111" s="16"/>
-    </row>
-    <row r="112" spans="1:7">
-      <c r="A112" s="16"/>
-      <c r="B112" s="14"/>
-      <c r="C112" s="15"/>
-      <c r="D112" s="16"/>
-      <c r="E112" s="14"/>
-      <c r="F112" s="15"/>
-      <c r="G112" s="16"/>
-    </row>
-    <row r="113" spans="1:7">
-      <c r="A113" s="16"/>
-      <c r="B113" s="14"/>
-      <c r="C113" s="15"/>
-      <c r="D113" s="16"/>
-      <c r="E113" s="14"/>
-      <c r="F113" s="15"/>
-      <c r="G113" s="16"/>
-    </row>
-    <row r="114" spans="1:7">
-      <c r="A114" s="16"/>
-      <c r="B114" s="14"/>
-      <c r="C114" s="15"/>
-      <c r="D114" s="16"/>
-      <c r="E114" s="14"/>
-      <c r="F114" s="15"/>
-      <c r="G114" s="16"/>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A42:B43"/>
-    <mergeCell ref="C42:G43"/>
-    <mergeCell ref="A79:B80"/>
-    <mergeCell ref="C79:G80"/>
+  <mergeCells count="4">
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="C5:G6"/>
-    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A3:G3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6574,1123 +5445,97 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A2:K114"/>
+  <dimension ref="A2:G8"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="18" customHeight="1">
-      <c r="A2" s="55" t="s">
+    <row r="2" spans="1:7" ht="18" customHeight="1">
+      <c r="A2" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="58"/>
+    </row>
+    <row r="3" spans="1:7" ht="18" customHeight="1">
+      <c r="A3" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A5" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="55"/>
+      <c r="C5" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+    </row>
+    <row r="7" spans="1:7" ht="25.5">
+      <c r="A7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="57"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
+      <c r="B7" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="18" customHeight="1">
-      <c r="A3" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-    </row>
-    <row r="5" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A5" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="49"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-    </row>
-    <row r="6" spans="1:11" ht="30.75" customHeight="1">
-      <c r="A6" s="45"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="52"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-    </row>
-    <row r="8" spans="1:11" ht="26.25">
-      <c r="A8" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-    </row>
-    <row r="9" spans="1:11" ht="15">
-      <c r="A9" s="16"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-    </row>
-    <row r="10" spans="1:11" ht="15">
-      <c r="A10" s="16"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16"/>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-      <c r="K10"/>
-    </row>
-    <row r="11" spans="1:11" ht="15">
-      <c r="A11" s="16"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="16"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-    </row>
-    <row r="12" spans="1:11" ht="15">
-      <c r="A12" s="16"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-    </row>
-    <row r="13" spans="1:11" ht="15">
-      <c r="A13" s="16"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-    </row>
-    <row r="14" spans="1:11" ht="15">
-      <c r="A14" s="16"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="16"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-      <c r="K14"/>
-    </row>
-    <row r="15" spans="1:11" ht="15">
-      <c r="A15" s="16"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-    </row>
-    <row r="16" spans="1:11" ht="15">
-      <c r="A16" s="16"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-    </row>
-    <row r="17" spans="1:11" ht="15">
-      <c r="A17" s="16"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="16"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
-      <c r="K17"/>
-    </row>
-    <row r="18" spans="1:11" ht="15">
-      <c r="A18" s="16"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
-      <c r="K18"/>
-    </row>
-    <row r="19" spans="1:11" ht="15">
-      <c r="A19" s="16"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="16"/>
-      <c r="H19"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-    </row>
-    <row r="20" spans="1:11" ht="15">
-      <c r="A20" s="16"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="16"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="16"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="16"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="16"/>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="16"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="16"/>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="16"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="16"/>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="16"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="16"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="16"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="16"/>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="16"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="16"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="16"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="16"/>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="16"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="16"/>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="16"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="16"/>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="16"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="16"/>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="16"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="16"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="16"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="16"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="16"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="16"/>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="16"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="16"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="16"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="16"/>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="16"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="16"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="16"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="16"/>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="16"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="16"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="16"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="16"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" s="44"/>
-      <c r="C42" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="49"/>
-    </row>
-    <row r="43" spans="1:7" ht="27" customHeight="1">
-      <c r="A43" s="45"/>
-      <c r="B43" s="46"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="51"/>
-      <c r="F43" s="51"/>
-      <c r="G43" s="52"/>
-    </row>
-    <row r="45" spans="1:7" ht="25.5">
-      <c r="A45" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="16"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="16"/>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="16"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="16"/>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="16"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="16"/>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="16"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="16"/>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="16"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="16"/>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="16"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="16"/>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="16"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="16"/>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" s="16"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="16"/>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="16"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="16"/>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" s="16"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="16"/>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" s="16"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="16"/>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57" s="16"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="15"/>
-      <c r="G57" s="16"/>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="16"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="16"/>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="16"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="16"/>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="16"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="16"/>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="16"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="15"/>
-      <c r="G61" s="16"/>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="16"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="15"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="15"/>
-      <c r="G62" s="16"/>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="16"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="15"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="16"/>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="16"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="15"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="15"/>
-      <c r="G64" s="16"/>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="16"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="16"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="15"/>
-      <c r="G65" s="16"/>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="16"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="16"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="16"/>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" s="16"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="15"/>
-      <c r="G67" s="16"/>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="16"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="16"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="15"/>
-      <c r="G68" s="16"/>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="16"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="15"/>
-      <c r="D69" s="16"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="15"/>
-      <c r="G69" s="16"/>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" s="16"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="15"/>
-      <c r="D70" s="16"/>
-      <c r="E70" s="14"/>
-      <c r="F70" s="15"/>
-      <c r="G70" s="16"/>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" s="16"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="15"/>
-      <c r="D71" s="16"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="15"/>
-      <c r="G71" s="16"/>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="16"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="15"/>
-      <c r="D72" s="16"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="15"/>
-      <c r="G72" s="16"/>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="A73" s="16"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="15"/>
-      <c r="D73" s="16"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="15"/>
-      <c r="G73" s="16"/>
-    </row>
-    <row r="74" spans="1:7">
-      <c r="A74" s="16"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="16"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="15"/>
-      <c r="G74" s="16"/>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="A75" s="16"/>
-      <c r="B75" s="14"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="16"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="15"/>
-      <c r="G75" s="16"/>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" s="16"/>
-      <c r="B76" s="14"/>
-      <c r="C76" s="15"/>
-      <c r="D76" s="16"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="15"/>
-      <c r="G76" s="16"/>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="A77" s="16"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="15"/>
-      <c r="D77" s="16"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="15"/>
-      <c r="G77" s="16"/>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="A79" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="B79" s="44"/>
-      <c r="C79" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="D79" s="48"/>
-      <c r="E79" s="48"/>
-      <c r="F79" s="48"/>
-      <c r="G79" s="49"/>
-    </row>
-    <row r="80" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A80" s="45"/>
-      <c r="B80" s="46"/>
-      <c r="C80" s="50"/>
-      <c r="D80" s="51"/>
-      <c r="E80" s="51"/>
-      <c r="F80" s="51"/>
-      <c r="G80" s="52"/>
-    </row>
-    <row r="82" spans="1:7" ht="25.5">
-      <c r="A82" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B82" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C82" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D82" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E82" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F82" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G82" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7">
-      <c r="A83" s="16"/>
-      <c r="B83" s="14"/>
-      <c r="C83" s="15"/>
-      <c r="D83" s="16"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="15"/>
-      <c r="G83" s="16"/>
-    </row>
-    <row r="84" spans="1:7">
-      <c r="A84" s="16"/>
-      <c r="B84" s="14"/>
-      <c r="C84" s="15"/>
-      <c r="D84" s="16"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="15"/>
-      <c r="G84" s="16"/>
-    </row>
-    <row r="85" spans="1:7">
-      <c r="A85" s="16"/>
-      <c r="B85" s="14"/>
-      <c r="C85" s="15"/>
-      <c r="D85" s="16"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="15"/>
-      <c r="G85" s="16"/>
-    </row>
-    <row r="86" spans="1:7">
-      <c r="A86" s="16"/>
-      <c r="B86" s="14"/>
-      <c r="C86" s="15"/>
-      <c r="D86" s="16"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="15"/>
-      <c r="G86" s="16"/>
-    </row>
-    <row r="87" spans="1:7">
-      <c r="A87" s="16"/>
-      <c r="B87" s="14"/>
-      <c r="C87" s="15"/>
-      <c r="D87" s="16"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="15"/>
-      <c r="G87" s="16"/>
-    </row>
-    <row r="88" spans="1:7">
-      <c r="A88" s="16"/>
-      <c r="B88" s="14"/>
-      <c r="C88" s="15"/>
-      <c r="D88" s="16"/>
-      <c r="E88" s="14"/>
-      <c r="F88" s="15"/>
-      <c r="G88" s="16"/>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="A89" s="16"/>
-      <c r="B89" s="14"/>
-      <c r="C89" s="15"/>
-      <c r="D89" s="16"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="15"/>
-      <c r="G89" s="16"/>
-    </row>
-    <row r="90" spans="1:7">
-      <c r="A90" s="16"/>
-      <c r="B90" s="14"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="16"/>
-      <c r="E90" s="14"/>
-      <c r="F90" s="15"/>
-      <c r="G90" s="16"/>
-    </row>
-    <row r="91" spans="1:7">
-      <c r="A91" s="16"/>
-      <c r="B91" s="14"/>
-      <c r="C91" s="15"/>
-      <c r="D91" s="16"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="15"/>
-      <c r="G91" s="16"/>
-    </row>
-    <row r="92" spans="1:7">
-      <c r="A92" s="16"/>
-      <c r="B92" s="14"/>
-      <c r="C92" s="15"/>
-      <c r="D92" s="16"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="15"/>
-      <c r="G92" s="16"/>
-    </row>
-    <row r="93" spans="1:7">
-      <c r="A93" s="16"/>
-      <c r="B93" s="14"/>
-      <c r="C93" s="15"/>
-      <c r="D93" s="16"/>
-      <c r="E93" s="14"/>
-      <c r="F93" s="15"/>
-      <c r="G93" s="16"/>
-    </row>
-    <row r="94" spans="1:7">
-      <c r="A94" s="16"/>
-      <c r="B94" s="14"/>
-      <c r="C94" s="15"/>
-      <c r="D94" s="16"/>
-      <c r="E94" s="14"/>
-      <c r="F94" s="15"/>
-      <c r="G94" s="16"/>
-    </row>
-    <row r="95" spans="1:7">
-      <c r="A95" s="16"/>
-      <c r="B95" s="14"/>
-      <c r="C95" s="15"/>
-      <c r="D95" s="16"/>
-      <c r="E95" s="14"/>
-      <c r="F95" s="15"/>
-      <c r="G95" s="16"/>
-    </row>
-    <row r="96" spans="1:7">
-      <c r="A96" s="16"/>
-      <c r="B96" s="14"/>
-      <c r="C96" s="15"/>
-      <c r="D96" s="16"/>
-      <c r="E96" s="14"/>
-      <c r="F96" s="15"/>
-      <c r="G96" s="16"/>
-    </row>
-    <row r="97" spans="1:7">
-      <c r="A97" s="16"/>
-      <c r="B97" s="14"/>
-      <c r="C97" s="15"/>
-      <c r="D97" s="16"/>
-      <c r="E97" s="14"/>
-      <c r="F97" s="15"/>
-      <c r="G97" s="16"/>
-    </row>
-    <row r="98" spans="1:7">
-      <c r="A98" s="16"/>
-      <c r="B98" s="14"/>
-      <c r="C98" s="15"/>
-      <c r="D98" s="16"/>
-      <c r="E98" s="14"/>
-      <c r="F98" s="15"/>
-      <c r="G98" s="16"/>
-    </row>
-    <row r="99" spans="1:7">
-      <c r="A99" s="16"/>
-      <c r="B99" s="14"/>
-      <c r="C99" s="15"/>
-      <c r="D99" s="16"/>
-      <c r="E99" s="14"/>
-      <c r="F99" s="15"/>
-      <c r="G99" s="16"/>
-    </row>
-    <row r="100" spans="1:7">
-      <c r="A100" s="16"/>
-      <c r="B100" s="14"/>
-      <c r="C100" s="15"/>
-      <c r="D100" s="16"/>
-      <c r="E100" s="14"/>
-      <c r="F100" s="15"/>
-      <c r="G100" s="16"/>
-    </row>
-    <row r="101" spans="1:7">
-      <c r="A101" s="16"/>
-      <c r="B101" s="14"/>
-      <c r="C101" s="15"/>
-      <c r="D101" s="16"/>
-      <c r="E101" s="14"/>
-      <c r="F101" s="15"/>
-      <c r="G101" s="16"/>
-    </row>
-    <row r="102" spans="1:7">
-      <c r="A102" s="16"/>
-      <c r="B102" s="14"/>
-      <c r="C102" s="15"/>
-      <c r="D102" s="16"/>
-      <c r="E102" s="14"/>
-      <c r="F102" s="15"/>
-      <c r="G102" s="16"/>
-    </row>
-    <row r="103" spans="1:7">
-      <c r="A103" s="16"/>
-      <c r="B103" s="14"/>
-      <c r="C103" s="15"/>
-      <c r="D103" s="16"/>
-      <c r="E103" s="14"/>
-      <c r="F103" s="15"/>
-      <c r="G103" s="16"/>
-    </row>
-    <row r="104" spans="1:7">
-      <c r="A104" s="16"/>
-      <c r="B104" s="14"/>
-      <c r="C104" s="15"/>
-      <c r="D104" s="16"/>
-      <c r="E104" s="14"/>
-      <c r="F104" s="15"/>
-      <c r="G104" s="16"/>
-    </row>
-    <row r="105" spans="1:7">
-      <c r="A105" s="16"/>
-      <c r="B105" s="14"/>
-      <c r="C105" s="15"/>
-      <c r="D105" s="16"/>
-      <c r="E105" s="14"/>
-      <c r="F105" s="15"/>
-      <c r="G105" s="16"/>
-    </row>
-    <row r="106" spans="1:7">
-      <c r="A106" s="16"/>
-      <c r="B106" s="14"/>
-      <c r="C106" s="15"/>
-      <c r="D106" s="16"/>
-      <c r="E106" s="14"/>
-      <c r="F106" s="15"/>
-      <c r="G106" s="16"/>
-    </row>
-    <row r="107" spans="1:7">
-      <c r="A107" s="16"/>
-      <c r="B107" s="14"/>
-      <c r="C107" s="15"/>
-      <c r="D107" s="16"/>
-      <c r="E107" s="14"/>
-      <c r="F107" s="15"/>
-      <c r="G107" s="16"/>
-    </row>
-    <row r="108" spans="1:7">
-      <c r="A108" s="16"/>
-      <c r="B108" s="14"/>
-      <c r="C108" s="15"/>
-      <c r="D108" s="16"/>
-      <c r="E108" s="14"/>
-      <c r="F108" s="15"/>
-      <c r="G108" s="16"/>
-    </row>
-    <row r="109" spans="1:7">
-      <c r="A109" s="16"/>
-      <c r="B109" s="14"/>
-      <c r="C109" s="15"/>
-      <c r="D109" s="16"/>
-      <c r="E109" s="14"/>
-      <c r="F109" s="15"/>
-      <c r="G109" s="16"/>
-    </row>
-    <row r="110" spans="1:7">
-      <c r="A110" s="16"/>
-      <c r="B110" s="14"/>
-      <c r="C110" s="15"/>
-      <c r="D110" s="16"/>
-      <c r="E110" s="14"/>
-      <c r="F110" s="15"/>
-      <c r="G110" s="16"/>
-    </row>
-    <row r="111" spans="1:7">
-      <c r="A111" s="16"/>
-      <c r="B111" s="14"/>
-      <c r="C111" s="15"/>
-      <c r="D111" s="16"/>
-      <c r="E111" s="14"/>
-      <c r="F111" s="15"/>
-      <c r="G111" s="16"/>
-    </row>
-    <row r="112" spans="1:7">
-      <c r="A112" s="16"/>
-      <c r="B112" s="14"/>
-      <c r="C112" s="15"/>
-      <c r="D112" s="16"/>
-      <c r="E112" s="14"/>
-      <c r="F112" s="15"/>
-      <c r="G112" s="16"/>
-    </row>
-    <row r="113" spans="1:7">
-      <c r="A113" s="16"/>
-      <c r="B113" s="14"/>
-      <c r="C113" s="15"/>
-      <c r="D113" s="16"/>
-      <c r="E113" s="14"/>
-      <c r="F113" s="15"/>
-      <c r="G113" s="16"/>
-    </row>
-    <row r="114" spans="1:7">
-      <c r="A114" s="16"/>
-      <c r="B114" s="14"/>
-      <c r="C114" s="15"/>
-      <c r="D114" s="16"/>
-      <c r="E114" s="14"/>
-      <c r="F114" s="15"/>
-      <c r="G114" s="16"/>
+    <row r="8" spans="1:7">
+      <c r="A8" s="25"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A79:B80"/>
-    <mergeCell ref="C79:G80"/>
+  <mergeCells count="4">
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="C5:G6"/>
-    <mergeCell ref="A42:B43"/>
-    <mergeCell ref="C42:G43"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="89" orientation="portrait" r:id="rId1"/>
@@ -7706,29 +5551,29 @@
   <dimension ref="A2:J11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
-    <col min="2" max="9" width="10.7109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="2" max="10" width="12.85546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
+      <c r="A2" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
     </row>
     <row r="3" spans="1:10" ht="18">
       <c r="A3" s="12"/>
@@ -7738,128 +5583,128 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="60"/>
+      <c r="B4" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="62"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:10" ht="24" customHeight="1">
-      <c r="B6" s="25">
+      <c r="B6" s="22">
         <v>2015</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="22">
         <v>2016</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="22">
         <v>2017</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="22">
         <v>2018</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="22">
         <v>2019</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="22">
         <v>2020</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="22">
         <v>2021</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="22">
         <v>2022</v>
       </c>
-      <c r="J6" s="25" t="s">
-        <v>55</v>
+      <c r="J6" s="22" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="24" customHeight="1">
-      <c r="A7" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="26">
+    <row r="7" spans="1:10" ht="41.25" customHeight="1">
+      <c r="A7" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="27">
         <v>0</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="27">
         <v>0</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="27">
         <v>0</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="27">
         <v>0</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="27">
         <v>0</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="27">
         <v>0</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="27">
         <v>0</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="27">
         <v>0</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="24" customHeight="1">
-      <c r="A8" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="26">
+    <row r="8" spans="1:10" ht="41.25" customHeight="1">
+      <c r="A8" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="27">
         <v>0</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="27">
         <v>0</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="27">
         <v>0</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="27">
         <v>0</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="27">
         <v>0</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="27">
         <v>0</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="27">
         <v>0</v>
       </c>
-      <c r="I8" s="26">
+      <c r="I8" s="27">
         <v>0</v>
       </c>
-      <c r="J8" s="26">
+      <c r="J8" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="24" customHeight="1">
-      <c r="A10" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="26">
+    <row r="10" spans="1:10" ht="41.25" customHeight="1">
+      <c r="A10" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="24" customHeight="1">
-      <c r="A11" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="26">
+    <row r="11" spans="1:10" ht="41.25" customHeight="1">
+      <c r="A11" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="28">
         <v>0</v>
       </c>
     </row>
@@ -7879,10 +5724,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A2:C30"/>
+  <dimension ref="A2:C7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7894,11 +5739,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="61" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
+      <c r="A2" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -7909,10 +5754,10 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="58" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="60"/>
+      <c r="B4" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="62"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -7920,135 +5765,20 @@
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="22" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="16"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="16"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="16"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="16"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="16"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="16"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="16"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="16"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="16"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="16"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="16"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="16"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="16"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="16"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="16"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
+      <c r="C7" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8066,10 +5796,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A2:B30"/>
+  <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8080,10 +5810,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="61"/>
+      <c r="B2" s="63"/>
     </row>
     <row r="3" spans="1:2" ht="18">
       <c r="A3" s="12"/>
@@ -8093,8 +5823,8 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>45</v>
+      <c r="B4" s="16" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -8102,108 +5832,16 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15"/>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="15"/>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="14"/>
-      <c r="B25" s="15"/>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="15"/>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="15"/>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="15"/>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="14"/>
-      <c r="B30" s="15"/>
+      <c r="B7" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8220,10 +5858,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A2:C30"/>
+  <dimension ref="A2:C7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8235,11 +5873,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="61" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
+      <c r="A2" s="63" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -8250,10 +5888,10 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="60"/>
+      <c r="B4" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="62"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -8261,135 +5899,20 @@
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>65</v>
+      <c r="C6" s="22" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="16"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="16"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="16"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="16"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="16"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="16"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="16"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="16"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="16"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="16"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="16"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="16"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="16"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="16"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="16"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
+      <c r="C7" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8407,10 +5930,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8426,37 +5949,37 @@
     <col min="9" max="9" width="17.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="24" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15" style="68" customWidth="1"/>
-    <col min="13" max="13" width="16" style="68" customWidth="1"/>
+    <col min="12" max="12" width="15" style="23" customWidth="1"/>
+    <col min="13" max="13" width="16" style="23" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1"/>
     <row r="2" spans="1:13" ht="18" customHeight="1">
-      <c r="A2" s="61" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
+      <c r="A2" s="63" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
     </row>
     <row r="4" spans="1:13" ht="20.25" customHeight="1">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="64"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="65" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E4" s="66"/>
       <c r="F4" s="66"/>
@@ -8468,226 +5991,68 @@
       <c r="L4" s="66"/>
       <c r="M4" s="67"/>
     </row>
-    <row r="6" spans="1:13" ht="53.25" customHeight="1">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:13" ht="39.75" customHeight="1">
+      <c r="A6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="17" t="s">
+      <c r="C6" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="17" t="s">
+      <c r="I6" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="69" t="s">
-        <v>59</v>
-      </c>
-      <c r="M6" s="69" t="s">
-        <v>60</v>
+      <c r="L6" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" s="26" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="16"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
       <c r="K7" s="14"/>
-      <c r="L7" s="70"/>
-      <c r="M7" s="71"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="71"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="70"/>
-      <c r="M9" s="71"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="70"/>
-      <c r="M10" s="71"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="70"/>
-      <c r="M11" s="71"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="70"/>
-      <c r="M12" s="71"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="70"/>
-      <c r="M13" s="71"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="70"/>
-      <c r="M14" s="71"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="70"/>
-      <c r="M15" s="71"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="70"/>
-      <c r="M16" s="71"/>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="70"/>
-      <c r="M17" s="71"/>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="70"/>
-      <c r="M18" s="71"/>
+      <c r="K8" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
updated template for lpi reports
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2333 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: efc4bd34bf0557623dccd2fdbe334e91ec12d52e
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmart\workspace64bitNew\SEMOSS_2014\export\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahkhalil\newWorkspace\Semoss\export\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="System Overview" sheetId="21" r:id="rId1"/>
@@ -805,6 +805,18 @@
     <xf numFmtId="44" fontId="10" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -838,20 +850,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5134,22 +5134,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="41" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="43"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="47"/>
     </row>
     <row r="3" spans="1:13" s="21" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="17"/>
@@ -5168,20 +5168,20 @@
     </row>
     <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
     </row>
     <row r="5" spans="1:13" ht="7.5" customHeight="1">
       <c r="A5" s="5"/>
@@ -5207,22 +5207,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="41" t="s">
+      <c r="C7" s="42"/>
+      <c r="D7" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="43"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="47"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -5233,65 +5233,67 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="48"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="35"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44" t="s">
+      <c r="C10" s="36"/>
+      <c r="D10" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="45"/>
-      <c r="F10" s="44" t="s">
+      <c r="E10" s="48"/>
+      <c r="F10" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="44"/>
-      <c r="H10" s="33" t="s">
+      <c r="G10" s="36"/>
+      <c r="H10" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="34"/>
-      <c r="J10" s="44" t="s">
+      <c r="I10" s="38"/>
+      <c r="J10" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44" t="s">
+      <c r="K10" s="36"/>
+      <c r="L10" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="44"/>
+      <c r="M10" s="36"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="36"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:M7"/>
     <mergeCell ref="B9:M9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="H10:I10"/>
@@ -5308,8 +5310,6 @@
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:M7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5447,7 +5447,7 @@
   </sheetPr>
   <dimension ref="A2:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -5932,8 +5932,8 @@
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6049,7 +6049,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="K8" s="30" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="L8" s="29"/>
       <c r="M8" s="29"/>

</xml_diff>

<commit_message>
updated SOR Report Table for LPI and LNPI individual system report
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2357 ef391c1c-ee15-45f7-b1d6-dde3d27a2169
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahkhalil\newWorkspace\Semoss\export\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmart\workspace64bitNew\SEMOSS_2014\export\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="System Overview" sheetId="21" r:id="rId1"/>
@@ -20,9 +20,9 @@
     <sheet name="Data Provenance" sheetId="28" r:id="rId6"/>
     <sheet name="DHMSM Data Requirements" sheetId="26" r:id="rId7"/>
     <sheet name="System Interfaces" sheetId="27" r:id="rId8"/>
+    <sheet name="System SOR" sheetId="30" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
@@ -30,6 +30,7 @@
     <externalReference r:id="rId14"/>
     <externalReference r:id="rId15"/>
     <externalReference r:id="rId16"/>
+    <externalReference r:id="rId17"/>
   </externalReferences>
   <definedNames>
     <definedName name="Additional">[1]Data!$D$3:$D$15</definedName>
@@ -54,6 +55,7 @@
     <definedName name="FY15_Total">'[2]Fiscal Year Breakdown'!$AO$18</definedName>
     <definedName name="I_O" localSheetId="3">#REF!</definedName>
     <definedName name="I_O" localSheetId="0">#REF!</definedName>
+    <definedName name="I_O" localSheetId="8">#REF!</definedName>
     <definedName name="I_O">#REF!</definedName>
     <definedName name="Link3">[4]Data1!$D$4:$D$182</definedName>
     <definedName name="MDM_Person">'[2]Detailed Planner - Enabler'!$K$86</definedName>
@@ -71,6 +73,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Software Lifecycles'!$7:$7</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'System Data'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="7">'System Interfaces'!$6:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="8">'System SOR'!$6:$6</definedName>
     <definedName name="Priority3">[4]Data1!$B$4:$B$6</definedName>
     <definedName name="ProcContractMonths">'[2]New Timeline'!$A$22</definedName>
     <definedName name="RangeBLU">[5]BLUBackEnd!$G$5:$G$49</definedName>
@@ -86,6 +89,7 @@
     <definedName name="Teams">[2]Cheat!$A$38:$A$39</definedName>
     <definedName name="Type" localSheetId="3">#REF!</definedName>
     <definedName name="Type" localSheetId="0">#REF!</definedName>
+    <definedName name="Type" localSheetId="8">#REF!</definedName>
     <definedName name="Type">#REF!</definedName>
     <definedName name="UDDI_ROI">[2]BOM!$N$58</definedName>
     <definedName name="xx">[8]Data!$E$3:$E$151</definedName>
@@ -96,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
   <si>
     <t>Garrison / Theater</t>
   </si>
@@ -326,6 +330,15 @@
       </rPr>
       <t>(expected @DATE@)</t>
     </r>
+  </si>
+  <si>
+    <t>System Source of Record</t>
+  </si>
+  <si>
+    <t>This section displays the data objects @SYSTEM@ is a source of record of and consumes as well as showing the number of low probability systems that @SYSTEM@ provides the data object to. It also shows the other systems that are a source of the data object and the number of low probability systems they provide data for.</t>
+  </si>
+  <si>
+    <t>Provided or Consumed</t>
   </si>
 </sst>
 </file>
@@ -725,7 +738,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -805,6 +818,42 @@
     <xf numFmtId="44" fontId="10" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -814,45 +863,12 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -909,6 +925,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -5134,22 +5159,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="45" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="47"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="42"/>
     </row>
     <row r="3" spans="1:13" s="21" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="17"/>
@@ -5168,20 +5193,20 @@
     </row>
     <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="44"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
     </row>
     <row r="5" spans="1:13" ht="7.5" customHeight="1">
       <c r="A5" s="5"/>
@@ -5207,22 +5232,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="45" t="s">
+      <c r="C7" s="37"/>
+      <c r="D7" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="47"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="42"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -5233,68 +5258,65 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="35"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="47"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36" t="s">
+      <c r="C10" s="43"/>
+      <c r="D10" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="48"/>
-      <c r="F10" s="36" t="s">
+      <c r="E10" s="44"/>
+      <c r="F10" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="37" t="s">
+      <c r="G10" s="43"/>
+      <c r="H10" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="38"/>
-      <c r="J10" s="36" t="s">
+      <c r="I10" s="49"/>
+      <c r="J10" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36" t="s">
+      <c r="K10" s="43"/>
+      <c r="L10" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="36"/>
+      <c r="M10" s="43"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="40"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="B11:C11"/>
@@ -5310,6 +5332,9 @@
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5346,26 +5371,26 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
@@ -5373,17 +5398,17 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="50" t="s">
+      <c r="B5" s="55"/>
+      <c r="C5" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="53"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
@@ -5464,39 +5489,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18" customHeight="1">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="59"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
     </row>
     <row r="5" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="59" t="s">
+      <c r="B5" s="56"/>
+      <c r="C5" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
     </row>
     <row r="7" spans="1:7" ht="25.5">
       <c r="A7" s="22" t="s">
@@ -5562,18 +5587,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
     </row>
     <row r="3" spans="1:10" ht="18">
       <c r="A3" s="12"/>
@@ -5583,17 +5608,17 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="63"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="2"/>
@@ -5739,11 +5764,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -5754,10 +5779,10 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="62"/>
+      <c r="C4" s="63"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -5810,10 +5835,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="63"/>
+      <c r="B2" s="64"/>
     </row>
     <row r="3" spans="1:2" ht="18">
       <c r="A3" s="12"/>
@@ -5873,11 +5898,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -5888,10 +5913,10 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="62"/>
+      <c r="C4" s="63"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -5932,7 +5957,7 @@
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
@@ -5956,40 +5981,40 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1"/>
     <row r="2" spans="1:13" ht="18" customHeight="1">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
     </row>
     <row r="4" spans="1:13" ht="20.25" customHeight="1">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="65" t="s">
+      <c r="B4" s="65"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="68"/>
     </row>
     <row r="6" spans="1:13" ht="39.75" customHeight="1">
       <c r="A6" s="15" t="s">
@@ -6064,4 +6089,78 @@
   <pageSetup scale="48" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="10" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18" customHeight="1"/>
+    <row r="2" spans="1:11" ht="18" customHeight="1">
+      <c r="A2" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+    </row>
+    <row r="4" spans="1:11" ht="53.25" customHeight="1">
+      <c r="A4" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="65"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="71"/>
+    </row>
+    <row r="6" spans="1:11" ht="39.75" customHeight="1">
+      <c r="A6" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:K4"/>
+    <mergeCell ref="A2:K2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="48" orientation="landscape" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated system transition report to include SOR
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2367 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 46cea2f5956a23f11b7c6b7ee325aac6bc2daab8
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -738,7 +738,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -821,6 +821,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -848,9 +857,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -863,12 +869,6 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -914,9 +914,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -933,6 +930,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5159,22 +5165,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="40" t="s">
+      <c r="C2" s="40"/>
+      <c r="D2" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="42"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="45"/>
     </row>
     <row r="3" spans="1:13" s="21" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="17"/>
@@ -5193,20 +5199,20 @@
     </row>
     <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
     </row>
     <row r="5" spans="1:13" ht="7.5" customHeight="1">
       <c r="A5" s="5"/>
@@ -5232,22 +5238,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="40" t="s">
+      <c r="C7" s="40"/>
+      <c r="D7" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="42"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="45"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -5258,65 +5264,67 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="46"/>
-      <c r="M9" s="47"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="49"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43" t="s">
+      <c r="C10" s="34"/>
+      <c r="D10" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="44"/>
-      <c r="F10" s="43" t="s">
+      <c r="E10" s="46"/>
+      <c r="F10" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="43"/>
-      <c r="H10" s="48" t="s">
+      <c r="G10" s="34"/>
+      <c r="H10" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="49"/>
-      <c r="J10" s="43" t="s">
+      <c r="I10" s="36"/>
+      <c r="J10" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43" t="s">
+      <c r="K10" s="34"/>
+      <c r="L10" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="43"/>
+      <c r="M10" s="34"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="35"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="B11:C11"/>
@@ -5333,8 +5341,6 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5957,8 +5963,8 @@
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5998,23 +6004,23 @@
       <c r="M2" s="64"/>
     </row>
     <row r="4" spans="1:13" ht="20.25" customHeight="1">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="66" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="68"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="67"/>
     </row>
     <row r="6" spans="1:13" ht="39.75" customHeight="1">
       <c r="A6" s="15" t="s">
@@ -6099,7 +6105,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -6125,21 +6131,21 @@
       <c r="K2" s="64"/>
     </row>
     <row r="4" spans="1:11" ht="53.25" customHeight="1">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="69" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="71"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="70"/>
     </row>
     <row r="6" spans="1:11" ht="39.75" customHeight="1">
       <c r="A6" s="22" t="s">

</xml_diff>

<commit_message>
changed tab name for lpi/lpni template
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2438 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 6bff4666ecf6ff00391fa9444c5c1627280743cb
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmart\workspace64bitNew\SEMOSS_2014\export\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahkhalil\newWorkspace\Semoss\export\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="727" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="31" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Hardware Lifecycles" sheetId="23" r:id="rId4"/>
     <sheet name="Modernization Timeline" sheetId="29" r:id="rId5"/>
     <sheet name="System Data" sheetId="30" r:id="rId6"/>
-    <sheet name="Data Provenance" sheetId="28" r:id="rId7"/>
+    <sheet name="SOR Overlap with DHMSM" sheetId="28" r:id="rId7"/>
     <sheet name="DHMSM Data Requirements" sheetId="26" r:id="rId8"/>
     <sheet name="System Interfaces" sheetId="27" r:id="rId9"/>
   </sheets>
@@ -71,10 +71,10 @@
     <definedName name="Portal_ROI">[2]BOM!$N$46</definedName>
     <definedName name="Portal_SUM">'[2]POM 2 Enabler - FY12'!$N$102</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'System Overview'!$A$2:$M$11</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="6">'Data Provenance'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="7">'DHMSM Data Requirements'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'Hardware Lifecycles'!$7:$7</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Software Lifecycles'!$7:$7</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="6">'SOR Overlap with DHMSM'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="5">'System Data'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="8">'System Interfaces'!$6:$6</definedName>
     <definedName name="Priority3">[5]Data1!$B$4:$B$6</definedName>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>Capability</t>
-  </si>
-  <si>
-    <t>Data Provenance</t>
   </si>
   <si>
     <t>Services</t>
@@ -389,6 +386,9 @@
       </rPr>
       <t xml:space="preserve"> at the top of the worksheet on how to complete that respective tab. </t>
     </r>
+  </si>
+  <si>
+    <t>SOR Overlap with DHMSM</t>
   </si>
 </sst>
 </file>
@@ -924,6 +924,18 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -951,20 +963,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1014,10 +1014,19 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1028,15 +1037,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -24357,12 +24357,12 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="32.25" customHeight="1">
       <c r="A2" s="40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
@@ -24378,12 +24378,12 @@
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="235.5" customHeight="1">
       <c r="A4" s="42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
@@ -24399,12 +24399,12 @@
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="32" customFormat="1" ht="29.25" customHeight="1">
       <c r="A6" s="40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
@@ -24420,12 +24420,12 @@
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="54.75" customHeight="1">
       <c r="A8" s="37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
@@ -24539,22 +24539,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="54"/>
+      <c r="D2" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="53"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="57"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -24574,7 +24574,7 @@
     <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="41"/>
       <c r="D4" s="41"/>
@@ -24612,22 +24612,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="49" t="s">
-        <v>31</v>
+      <c r="B7" s="53" t="s">
+        <v>30</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51" t="s">
-        <v>38</v>
+      <c r="C7" s="54"/>
+      <c r="D7" s="55" t="s">
+        <v>37</v>
       </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="53"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="57"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -24638,65 +24638,67 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="57"/>
-      <c r="L9" s="57"/>
-      <c r="M9" s="58"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="47"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54" t="s">
+      <c r="C10" s="48"/>
+      <c r="D10" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="55"/>
-      <c r="F10" s="54" t="s">
+      <c r="E10" s="58"/>
+      <c r="F10" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="48"/>
+      <c r="H10" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="54"/>
-      <c r="H10" s="45" t="s">
+      <c r="I10" s="50"/>
+      <c r="J10" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="I10" s="46"/>
-      <c r="J10" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54" t="s">
+      <c r="K10" s="48"/>
+      <c r="L10" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="54"/>
+      <c r="M10" s="48"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="48"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:M7"/>
     <mergeCell ref="B9:M9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="H10:I10"/>
@@ -24713,8 +24715,6 @@
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:M7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24747,12 +24747,12 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
       <c r="A2" s="59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
@@ -24763,7 +24763,7 @@
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
       <c r="A3" s="65" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="65"/>
       <c r="C3" s="65"/>
@@ -24774,16 +24774,16 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18.75" customHeight="1">
       <c r="A5" s="63" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="64"/>
       <c r="C5" s="60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="61"/>
       <c r="E5" s="61"/>
@@ -24792,30 +24792,30 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="25.5">
       <c r="A7" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="35" t="s">
+      <c r="E7" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="F7" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="35" t="s">
-        <v>21</v>
-      </c>
       <c r="G7" s="35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -24829,7 +24829,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -24870,7 +24870,7 @@
   <sheetData>
     <row r="2" spans="1:7" ht="18" customHeight="1">
       <c r="A2" s="66" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="67"/>
       <c r="C2" s="67"/>
@@ -24892,11 +24892,11 @@
     </row>
     <row r="5" spans="1:7" ht="18.75" customHeight="1">
       <c r="A5" s="65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="65"/>
       <c r="C5" s="69" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="69"/>
       <c r="E5" s="69"/>
@@ -24905,25 +24905,25 @@
     </row>
     <row r="7" spans="1:7" ht="25.5">
       <c r="A7" s="35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="F7" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="35" t="s">
-        <v>21</v>
-      </c>
       <c r="G7" s="35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -24968,7 +24968,7 @@
   <sheetData>
     <row r="2" spans="1:10" ht="18" customHeight="1">
       <c r="A2" s="73" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="73"/>
       <c r="C2" s="73"/>
@@ -24989,7 +24989,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="70" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="71"/>
       <c r="D4" s="71"/>
@@ -25030,12 +25030,12 @@
         <v>2022</v>
       </c>
       <c r="J6" s="35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="41.25" customHeight="1">
       <c r="A7" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="24">
         <v>0</v>
@@ -25067,7 +25067,7 @@
     </row>
     <row r="8" spans="1:10" ht="41.25" customHeight="1">
       <c r="A8" s="35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="24">
         <v>0</v>
@@ -25099,7 +25099,7 @@
     </row>
     <row r="10" spans="1:10" ht="41.25" customHeight="1">
       <c r="A10" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="25">
         <v>0</v>
@@ -25107,7 +25107,7 @@
     </row>
     <row r="11" spans="1:10" ht="41.25" customHeight="1">
       <c r="A11" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="25">
         <v>0</v>
@@ -25131,7 +25131,7 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -25146,7 +25146,7 @@
     <row r="1" spans="1:10" ht="18" customHeight="1"/>
     <row r="2" spans="1:10" ht="18" customHeight="1">
       <c r="A2" s="73" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="73"/>
       <c r="C2" s="73"/>
@@ -25162,24 +25162,24 @@
       <c r="A4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="80" t="s">
-        <v>59</v>
+      <c r="B4" s="75"/>
+      <c r="C4" s="76" t="s">
+        <v>58</v>
       </c>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="82"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="78"/>
     </row>
     <row r="6" spans="1:10" ht="39.75" customHeight="1">
       <c r="A6" s="35" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -25205,8 +25205,8 @@
   </sheetPr>
   <dimension ref="A2:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -25218,7 +25218,7 @@
   <sheetData>
     <row r="2" spans="1:2" ht="18">
       <c r="A2" s="73" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="B2" s="73"/>
     </row>
@@ -25231,7 +25231,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -25281,7 +25281,7 @@
   <sheetData>
     <row r="2" spans="1:3" ht="18">
       <c r="A2" s="73" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="73"/>
       <c r="C2" s="73"/>
@@ -25296,7 +25296,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="70" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="72"/>
     </row>
@@ -25313,7 +25313,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -25364,7 +25364,7 @@
     <row r="1" spans="1:13" ht="18" customHeight="1"/>
     <row r="2" spans="1:13" ht="18" customHeight="1">
       <c r="A2" s="73" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="73"/>
       <c r="C2" s="73"/>
@@ -25383,60 +25383,60 @@
       <c r="A4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="77" t="s">
-        <v>46</v>
+      <c r="B4" s="79"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="80" t="s">
+        <v>45</v>
       </c>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="79"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="82"/>
     </row>
     <row r="6" spans="1:13" ht="39.75" customHeight="1">
       <c r="A6" s="35" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="H6" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="35" t="s">
+      <c r="I6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="35" t="s">
-        <v>16</v>
-      </c>
       <c r="L6" s="36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M6" s="36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -25456,7 +25456,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="K8" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L8" s="26"/>
       <c r="M8" s="26"/>

</xml_diff>

<commit_message>
updated template for lpi/lpni report
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2441 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: e0c3867d9b645a52e42969c5244ffb3e33de7e16
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="31" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Hardware Lifecycles" sheetId="23" r:id="rId4"/>
     <sheet name="Modernization Timeline" sheetId="29" r:id="rId5"/>
     <sheet name="System Data" sheetId="30" r:id="rId6"/>
-    <sheet name="SOR Overlap with DHMSM" sheetId="28" r:id="rId7"/>
+    <sheet name="SOR Overlap With DHMSM" sheetId="28" r:id="rId7"/>
     <sheet name="DHMSM Data Requirements" sheetId="26" r:id="rId8"/>
     <sheet name="System Interfaces" sheetId="27" r:id="rId9"/>
   </sheets>
@@ -74,7 +74,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="7">'DHMSM Data Requirements'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'Hardware Lifecycles'!$7:$7</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Software Lifecycles'!$7:$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="6">'SOR Overlap with DHMSM'!$6:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="6">'SOR Overlap With DHMSM'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="5">'System Data'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="8">'System Interfaces'!$6:$6</definedName>
     <definedName name="Priority3">[5]Data1!$B$4:$B$6</definedName>
@@ -924,24 +924,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -963,7 +945,25 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -24539,22 +24539,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="55" t="s">
+      <c r="C2" s="48"/>
+      <c r="D2" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="57"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="51"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -24612,22 +24612,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="55" t="s">
+      <c r="C7" s="48"/>
+      <c r="D7" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="57"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="51"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -24638,68 +24638,65 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="46"/>
-      <c r="M9" s="47"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="56"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48" t="s">
+      <c r="C10" s="52"/>
+      <c r="D10" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="58"/>
-      <c r="F10" s="48" t="s">
+      <c r="E10" s="53"/>
+      <c r="F10" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="48"/>
-      <c r="H10" s="49" t="s">
+      <c r="G10" s="52"/>
+      <c r="H10" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="50"/>
-      <c r="J10" s="48" t="s">
+      <c r="I10" s="58"/>
+      <c r="J10" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48" t="s">
+      <c r="K10" s="52"/>
+      <c r="L10" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="48"/>
+      <c r="M10" s="52"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="52"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="B11:C11"/>
@@ -24715,6 +24712,9 @@
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25206,7 +25206,7 @@
   <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>